<commit_message>
V 0.55-B55 (final release) - Add VNAV Button (when using WASM module) - Add Item TOD (TopOfDescend for VNAV support) - Add Move Bar/Tile to next screen (Monitor) with RShift+RCtrl+Break - Add Using the Facility DB for Aiport Management (replacing the FS20_AptLib) - Add Check if the Facility DB is available and pop a msg box if not - Add Performance Tab and Notes Tab to FlightBag - Add Touchdown log (MyDocuments\MSFS_HudBarSave\TouchDownLog.csv) to FlightBag - Update AP Settings allow for large change on the left side of the item field (mouse wheel) - Update AltHold readout is FL when STD BARO is set or above 18000ft - Fix Bar/Window Location was not stored for profiles 5..10 - Cleanup of all new features - Disable SimConnect.cfg (as per MS it is only needed when connecting MSFS via Network) - SU10 compatibility checks - Moved to Visual Studio 2022 Community Edition - Update QuickGuides
</commit_message>
<xml_diff>
--- a/FS20_HudBar/Config/EngineMerge.xlsx
+++ b/FS20_HudBar/Config/EngineMerge.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4438" uniqueCount="296">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4518" uniqueCount="298">
   <si>
     <t>ACFT</t>
   </si>
@@ -906,6 +906,12 @@
   </si>
   <si>
     <t>ADF1_F</t>
+  </si>
+  <si>
+    <t>AP_VNAV</t>
+  </si>
+  <si>
+    <t>GPS_TOD</t>
   </si>
 </sst>
 </file>
@@ -7099,10 +7105,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:EK40"/>
+  <dimension ref="A1:EM40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="EL34" sqref="EL34"/>
+    <sheetView tabSelected="1" topLeftCell="T1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="EE38" sqref="EE38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7110,11 +7116,11 @@
     <col min="1" max="75" width="3.7109375" bestFit="1" customWidth="1"/>
     <col min="76" max="77" width="3.7109375" customWidth="1"/>
     <col min="78" max="86" width="3.7109375" bestFit="1" customWidth="1"/>
-    <col min="87" max="140" width="3.7109375" customWidth="1"/>
-    <col min="141" max="141" width="36.28515625" customWidth="1"/>
+    <col min="87" max="142" width="3.7109375" customWidth="1"/>
+    <col min="143" max="143" width="36.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:141" s="11" customFormat="1" ht="72" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:143" s="11" customFormat="1" ht="72" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>95</v>
       </c>
@@ -7533,13 +7539,19 @@
         <v>295</v>
       </c>
       <c r="EJ1" s="11" t="s">
+        <v>296</v>
+      </c>
+      <c r="EK1" s="11" t="s">
+        <v>297</v>
+      </c>
+      <c r="EL1" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="EK1" t="s">
+      <c r="EM1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:141" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:143" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>88</v>
       </c>
@@ -7993,14 +8005,20 @@
         <v>88</v>
       </c>
       <c r="EJ2" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EK2" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EL2" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EK2" t="str">
+      <c r="EM2" t="str">
         <f>Tabelle1!AS2</f>
         <v>Airbus A320 Neo</v>
       </c>
     </row>
-    <row r="3" spans="1:141" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:143" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
         <v>88</v>
       </c>
@@ -8454,14 +8472,20 @@
         <v>88</v>
       </c>
       <c r="EJ3" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EK3" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EL3" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EK3" t="str">
+      <c r="EM3" t="str">
         <f>Tabelle1!AS3</f>
         <v>Boeing 747-8i</v>
       </c>
     </row>
-    <row r="4" spans="1:141" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:143" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
         <v>88</v>
       </c>
@@ -8915,14 +8939,20 @@
         <v>88</v>
       </c>
       <c r="EJ4" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EK4" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EL4" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EK4" t="str">
+      <c r="EM4" t="str">
         <f>Tabelle1!AS4</f>
         <v>Boeing 787-10</v>
       </c>
     </row>
-    <row r="5" spans="1:141" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:143" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>88</v>
       </c>
@@ -9376,14 +9406,20 @@
         <v>88</v>
       </c>
       <c r="EJ5" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EK5" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EL5" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EK5" t="str">
+      <c r="EM5" t="str">
         <f>Tabelle1!AS5</f>
         <v>Boeing F/A 18E Super Hornet</v>
       </c>
     </row>
-    <row r="6" spans="1:141" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:143" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>88</v>
       </c>
@@ -9837,14 +9873,20 @@
         <v>88</v>
       </c>
       <c r="EJ6" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EK6" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EL6" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EK6" t="str">
+      <c r="EM6" t="str">
         <f>Tabelle1!AS6</f>
         <v>Baron G58</v>
       </c>
     </row>
-    <row r="7" spans="1:141" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:143" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>88</v>
       </c>
@@ -10298,14 +10340,20 @@
         <v>88</v>
       </c>
       <c r="EJ7" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EK7" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EL7" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EK7" t="str">
+      <c r="EM7" t="str">
         <f>Tabelle1!AS7</f>
         <v>Bonanza G36</v>
       </c>
     </row>
-    <row r="8" spans="1:141" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:143" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>88</v>
       </c>
@@ -10759,14 +10807,20 @@
         <v>88</v>
       </c>
       <c r="EJ8" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EK8" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EL8" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EK8" t="str">
+      <c r="EM8" t="str">
         <f>Tabelle1!AS8</f>
         <v>Beechcraft King Air 350i</v>
       </c>
     </row>
-    <row r="9" spans="1:141" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:143" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>88</v>
       </c>
@@ -11220,14 +11274,20 @@
         <v>88</v>
       </c>
       <c r="EJ9" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EK9" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EL9" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EK9" t="str">
+      <c r="EM9" t="str">
         <f>Tabelle1!AS9</f>
         <v>Cessna 152</v>
       </c>
     </row>
-    <row r="10" spans="1:141" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:143" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
         <v>88</v>
       </c>
@@ -11681,14 +11741,20 @@
         <v>88</v>
       </c>
       <c r="EJ10" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EK10" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EL10" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EK10" t="str">
+      <c r="EM10" t="str">
         <f>Tabelle1!AS10</f>
         <v>Cessna 152 Aero</v>
       </c>
     </row>
-    <row r="11" spans="1:141" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:143" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
         <v>88</v>
       </c>
@@ -12142,14 +12208,20 @@
         <v>88</v>
       </c>
       <c r="EJ11" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EK11" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EL11" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EK11" t="str">
+      <c r="EM11" t="str">
         <f>Tabelle1!AS11</f>
         <v>Cessna 172sp Skyhawk G1000</v>
       </c>
     </row>
-    <row r="12" spans="1:141" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:143" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
         <v>88</v>
       </c>
@@ -12603,14 +12675,20 @@
         <v>88</v>
       </c>
       <c r="EJ12" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EK12" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EL12" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EK12" t="str">
+      <c r="EM12" t="str">
         <f>Tabelle1!AS12</f>
         <v>Cessna 172sp Skyhawk</v>
       </c>
     </row>
-    <row r="13" spans="1:141" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:143" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
         <v>88</v>
       </c>
@@ -13064,14 +13142,20 @@
         <v>88</v>
       </c>
       <c r="EJ13" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EK13" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EL13" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EK13" t="str">
+      <c r="EM13" t="str">
         <f>Tabelle1!AS13</f>
         <v>Cessna 208B Grand Caravan EX</v>
       </c>
     </row>
-    <row r="14" spans="1:141" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:143" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
         <v>88</v>
       </c>
@@ -13525,14 +13609,20 @@
         <v>88</v>
       </c>
       <c r="EJ14" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EK14" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EL14" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EK14" t="str">
+      <c r="EM14" t="str">
         <f>Tabelle1!AS14</f>
         <v>Cessna CJ4 Citation</v>
       </c>
     </row>
-    <row r="15" spans="1:141" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:143" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
         <v>88</v>
       </c>
@@ -13986,14 +14076,20 @@
         <v>88</v>
       </c>
       <c r="EJ15" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EK15" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EL15" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EK15" t="str">
+      <c r="EM15" t="str">
         <f>Tabelle1!AS15</f>
         <v>Cessna Longitude</v>
       </c>
     </row>
-    <row r="16" spans="1:141" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:143" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
         <v>88</v>
       </c>
@@ -14447,14 +14543,20 @@
         <v>88</v>
       </c>
       <c r="EJ16" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EK16" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EL16" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EK16" t="str">
+      <c r="EM16" t="str">
         <f>Tabelle1!AS16</f>
         <v>DA40-NG</v>
       </c>
     </row>
-    <row r="17" spans="1:141" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:143" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
         <v>88</v>
       </c>
@@ -14908,14 +15010,20 @@
         <v>88</v>
       </c>
       <c r="EJ17" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EK17" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EL17" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EK17" t="str">
+      <c r="EM17" t="str">
         <f>Tabelle1!AS17</f>
         <v>DA40 TDI</v>
       </c>
     </row>
-    <row r="18" spans="1:141" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:143" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
         <v>88</v>
       </c>
@@ -15369,14 +15477,20 @@
         <v>88</v>
       </c>
       <c r="EJ18" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EK18" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EL18" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EK18" t="str">
+      <c r="EM18" t="str">
         <f>Tabelle1!AS18</f>
         <v>DA62</v>
       </c>
     </row>
-    <row r="19" spans="1:141" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:143" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
         <v>88</v>
       </c>
@@ -15830,14 +15944,20 @@
         <v>88</v>
       </c>
       <c r="EJ19" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EK19" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EL19" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EK19" t="str">
+      <c r="EM19" t="str">
         <f>Tabelle1!AS19</f>
         <v>DR400</v>
       </c>
     </row>
-    <row r="20" spans="1:141" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:143" x14ac:dyDescent="0.25">
       <c r="A20" s="12" t="s">
         <v>88</v>
       </c>
@@ -16291,14 +16411,20 @@
         <v>88</v>
       </c>
       <c r="EJ20" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EK20" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EL20" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EK20" t="str">
+      <c r="EM20" t="str">
         <f>Tabelle1!AS20</f>
         <v>DV20</v>
       </c>
     </row>
-    <row r="21" spans="1:141" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:143" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
         <v>88</v>
       </c>
@@ -16752,14 +16878,20 @@
         <v>88</v>
       </c>
       <c r="EJ21" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EK21" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EL21" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EK21" t="str">
+      <c r="EM21" t="str">
         <f>Tabelle1!AS21</f>
         <v>Extra 330</v>
       </c>
     </row>
-    <row r="22" spans="1:141" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:143" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="s">
         <v>88</v>
       </c>
@@ -17213,14 +17345,20 @@
         <v>88</v>
       </c>
       <c r="EJ22" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EK22" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EL22" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EK22" t="str">
+      <c r="EM22" t="str">
         <f>Tabelle1!AS22</f>
         <v>FlightDesignCT</v>
       </c>
     </row>
-    <row r="23" spans="1:141" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:143" x14ac:dyDescent="0.25">
       <c r="A23" s="12" t="s">
         <v>88</v>
       </c>
@@ -17674,14 +17812,20 @@
         <v>88</v>
       </c>
       <c r="EJ23" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EK23" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EL23" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EK23" t="str">
+      <c r="EM23" t="str">
         <f>Tabelle1!AS23</f>
         <v>Icon A5</v>
       </c>
     </row>
-    <row r="24" spans="1:141" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:143" x14ac:dyDescent="0.25">
       <c r="A24" s="12" t="s">
         <v>88</v>
       </c>
@@ -18135,14 +18279,20 @@
         <v>88</v>
       </c>
       <c r="EJ24" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EK24" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EL24" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EK24" t="str">
+      <c r="EM24" t="str">
         <f>Tabelle1!AS24</f>
         <v>Mudry Cap 10 C</v>
       </c>
     </row>
-    <row r="25" spans="1:141" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:143" x14ac:dyDescent="0.25">
       <c r="A25" s="12" t="s">
         <v>88</v>
       </c>
@@ -18596,14 +18746,20 @@
         <v>88</v>
       </c>
       <c r="EJ25" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EK25" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EL25" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EK25" t="str">
+      <c r="EM25" t="str">
         <f>Tabelle1!AS25</f>
         <v>Pilatus PC-6 Gauge</v>
       </c>
     </row>
-    <row r="26" spans="1:141" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:143" x14ac:dyDescent="0.25">
       <c r="A26" s="12" t="s">
         <v>88</v>
       </c>
@@ -19057,14 +19213,20 @@
         <v>88</v>
       </c>
       <c r="EJ26" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EK26" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EL26" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EK26" t="str">
+      <c r="EM26" t="str">
         <f>Tabelle1!AS26</f>
         <v>Pilatus PC-6 G950</v>
       </c>
     </row>
-    <row r="27" spans="1:141" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:143" x14ac:dyDescent="0.25">
       <c r="A27" s="12" t="s">
         <v>88</v>
       </c>
@@ -19518,14 +19680,20 @@
         <v>88</v>
       </c>
       <c r="EJ27" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EK27" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EL27" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EK27" t="str">
+      <c r="EM27" t="str">
         <f>Tabelle1!AS27</f>
         <v>Pipistrel Alpha Electro</v>
       </c>
     </row>
-    <row r="28" spans="1:141" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:143" x14ac:dyDescent="0.25">
       <c r="A28" s="12" t="s">
         <v>88</v>
       </c>
@@ -19979,14 +20147,20 @@
         <v>88</v>
       </c>
       <c r="EJ28" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EK28" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EL28" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EK28" t="str">
+      <c r="EM28" t="str">
         <f>Tabelle1!AS28</f>
         <v>Pitts Special 1S</v>
       </c>
     </row>
-    <row r="29" spans="1:141" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:143" x14ac:dyDescent="0.25">
       <c r="A29" s="12" t="s">
         <v>88</v>
       </c>
@@ -20440,14 +20614,20 @@
         <v>88</v>
       </c>
       <c r="EJ29" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EK29" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EL29" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EK29" t="str">
+      <c r="EM29" t="str">
         <f>Tabelle1!AS29</f>
         <v>Pitts Special S2S</v>
       </c>
     </row>
-    <row r="30" spans="1:141" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:143" x14ac:dyDescent="0.25">
       <c r="A30" s="12" t="s">
         <v>88</v>
       </c>
@@ -20901,14 +21081,20 @@
         <v>88</v>
       </c>
       <c r="EJ30" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EK30" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EL30" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EK30" t="str">
+      <c r="EM30" t="str">
         <f>Tabelle1!AS30</f>
         <v>Savage Cub</v>
       </c>
     </row>
-    <row r="31" spans="1:141" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:143" x14ac:dyDescent="0.25">
       <c r="A31" s="12" t="s">
         <v>88</v>
       </c>
@@ -21362,14 +21548,20 @@
         <v>88</v>
       </c>
       <c r="EJ31" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EK31" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EL31" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EK31" t="str">
+      <c r="EM31" t="str">
         <f>Tabelle1!AS31</f>
         <v>Savage Shock Ultra</v>
       </c>
     </row>
-    <row r="32" spans="1:141" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:143" x14ac:dyDescent="0.25">
       <c r="A32" s="12" t="s">
         <v>88</v>
       </c>
@@ -21823,14 +22015,20 @@
         <v>88</v>
       </c>
       <c r="EJ32" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EK32" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EL32" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EK32" t="str">
+      <c r="EM32" t="str">
         <f>Tabelle1!AS32</f>
         <v>SR22</v>
       </c>
     </row>
-    <row r="33" spans="1:141" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:143" x14ac:dyDescent="0.25">
       <c r="A33" s="12" t="s">
         <v>88</v>
       </c>
@@ -22284,14 +22482,20 @@
         <v>88</v>
       </c>
       <c r="EJ33" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EK33" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EL33" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EK33" t="str">
+      <c r="EM33" t="str">
         <f>Tabelle1!AS33</f>
         <v>TBM 930</v>
       </c>
     </row>
-    <row r="34" spans="1:141" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:143" x14ac:dyDescent="0.25">
       <c r="A34" s="12" t="s">
         <v>88</v>
       </c>
@@ -22745,14 +22949,20 @@
         <v>88</v>
       </c>
       <c r="EJ34" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EK34" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EL34" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EK34" t="str">
+      <c r="EM34" t="str">
         <f>Tabelle1!AS34</f>
         <v>Vertigo</v>
       </c>
     </row>
-    <row r="35" spans="1:141" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:143" x14ac:dyDescent="0.25">
       <c r="A35" s="12" t="s">
         <v>88</v>
       </c>
@@ -23206,14 +23416,20 @@
         <v>88</v>
       </c>
       <c r="EJ35" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EK35" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EL35" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EK35" t="str">
+      <c r="EM35" t="str">
         <f>Tabelle1!AS35</f>
         <v>VL3</v>
       </c>
     </row>
-    <row r="36" spans="1:141" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:143" x14ac:dyDescent="0.25">
       <c r="A36" s="12" t="s">
         <v>88</v>
       </c>
@@ -23667,14 +23883,20 @@
         <v>88</v>
       </c>
       <c r="EJ36" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EK36" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EL36" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EK36" t="str">
+      <c r="EM36" t="str">
         <f>Tabelle1!AS36</f>
         <v>Volocity</v>
       </c>
     </row>
-    <row r="37" spans="1:141" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:143" x14ac:dyDescent="0.25">
       <c r="A37" s="12" t="s">
         <v>88</v>
       </c>
@@ -24128,14 +24350,20 @@
         <v>88</v>
       </c>
       <c r="EJ37" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EK37" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EL37" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EK37" t="str">
+      <c r="EM37" t="str">
         <f>Tabelle1!AS37</f>
         <v>NXCub</v>
       </c>
     </row>
-    <row r="38" spans="1:141" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:143" x14ac:dyDescent="0.25">
       <c r="A38" s="12" t="s">
         <v>88</v>
       </c>
@@ -24589,14 +24817,20 @@
         <v>88</v>
       </c>
       <c r="EJ38" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EK38" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EL38" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EK38" t="str">
+      <c r="EM38" t="str">
         <f>Tabelle1!AS38</f>
         <v>XCub</v>
       </c>
     </row>
-    <row r="39" spans="1:141" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:143" x14ac:dyDescent="0.25">
       <c r="A39" s="12" t="s">
         <v>88</v>
       </c>
@@ -25050,14 +25284,20 @@
         <v>88</v>
       </c>
       <c r="EJ39" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EK39" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EL39" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EK39" t="str">
+      <c r="EM39" t="str">
         <f>Tabelle1!AS39</f>
         <v>SWS Kodiak 100 II</v>
       </c>
     </row>
-    <row r="40" spans="1:141" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:143" x14ac:dyDescent="0.25">
       <c r="A40" s="12" t="s">
         <v>88</v>
       </c>
@@ -25511,9 +25751,15 @@
         <v>88</v>
       </c>
       <c r="EJ40" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EK40" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EL40" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EK40" t="str">
+      <c r="EM40" t="str">
         <f>Tabelle1!AS40</f>
         <v>Generic Glider</v>
       </c>

</xml_diff>

<commit_message>
V 0.56-B56 - for testing - Add Color Config for Labels and Values - Add Audio Output Device selector in Configuration Dialog - Add SimOnGround indication (RA Label turns active - green - when on ground) - Add RAv voice out - touchdown indication - Add Re-Order command in the Config context menu for each column - Add Netto Variometer items (available when supported by the acft) - Add MacCrady Speed and Setting (available when supported by the acft) - Update Use SU11 Glider TE variometer when supported - Update Spoiler voice out (up-> retracted; down-> out) - Update Convert HudBar Settings to new Settings Concept - Update Appearance Name for Dark is now Inverse - SU11 compatibility checks - Fix Facility Data Loader issue found in SU11 - Update QuickGuides
</commit_message>
<xml_diff>
--- a/FS20_HudBar/Config/EngineMerge.xlsx
+++ b/FS20_HudBar/Config/EngineMerge.xlsx
@@ -11,14 +11,14 @@
     <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$A$1:$AS$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$A$1:$AU$1</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4518" uniqueCount="298">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4642" uniqueCount="303">
   <si>
     <t>ACFT</t>
   </si>
@@ -912,6 +912,21 @@
   </si>
   <si>
     <t>GPS_TOD</t>
+  </si>
+  <si>
+    <t>NETTO_MPS</t>
+  </si>
+  <si>
+    <t>NETTO_KTS</t>
+  </si>
+  <si>
+    <t>NETTO_ANI</t>
+  </si>
+  <si>
+    <t>MCRAD_MPS</t>
+  </si>
+  <si>
+    <t>MCRAD_KT</t>
   </si>
 </sst>
 </file>
@@ -1438,10 +1453,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AT42"/>
+  <dimension ref="A1:AV42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="AQ3" sqref="AQ3"/>
+      <selection activeCell="AU12" sqref="AU12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1454,11 +1469,11 @@
     <col min="7" max="31" width="3.7109375" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="3.28515625" customWidth="1"/>
     <col min="33" max="39" width="3.7109375" bestFit="1" customWidth="1"/>
-    <col min="40" max="44" width="3.7109375" customWidth="1"/>
-    <col min="45" max="46" width="36.28515625" customWidth="1"/>
+    <col min="40" max="46" width="3.7109375" customWidth="1"/>
+    <col min="47" max="48" width="36.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:46" s="11" customFormat="1" ht="57" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:48" s="11" customFormat="1" ht="64.5" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
@@ -1591,14 +1606,20 @@
       <c r="AR1" s="31" t="s">
         <v>275</v>
       </c>
-      <c r="AS1" s="11" t="s">
+      <c r="AS1" s="31" t="s">
+        <v>298</v>
+      </c>
+      <c r="AT1" s="31" t="s">
+        <v>301</v>
+      </c>
+      <c r="AU1" s="11" t="s">
         <v>220</v>
       </c>
-      <c r="AT1" s="11" t="s">
+      <c r="AV1" s="11" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>20</v>
       </c>
@@ -1732,14 +1753,20 @@
       <c r="AR2" s="32">
         <v>0</v>
       </c>
-      <c r="AS2" t="s">
+      <c r="AS2" s="32">
+        <v>0</v>
+      </c>
+      <c r="AT2" s="32">
+        <v>0</v>
+      </c>
+      <c r="AU2" t="s">
         <v>196</v>
       </c>
-      <c r="AT2" t="s">
+      <c r="AV2" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="3" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>22</v>
       </c>
@@ -1873,14 +1900,20 @@
       <c r="AR3" s="32">
         <v>0</v>
       </c>
-      <c r="AS3" t="s">
+      <c r="AS3" s="32">
+        <v>0</v>
+      </c>
+      <c r="AT3" s="32">
+        <v>0</v>
+      </c>
+      <c r="AU3" t="s">
         <v>198</v>
       </c>
-      <c r="AT3" t="s">
+      <c r="AV3" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="4" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>21</v>
       </c>
@@ -2014,14 +2047,20 @@
       <c r="AR4" s="32">
         <v>0</v>
       </c>
-      <c r="AS4" t="s">
+      <c r="AS4" s="32">
+        <v>0</v>
+      </c>
+      <c r="AT4" s="32">
+        <v>0</v>
+      </c>
+      <c r="AU4" t="s">
         <v>197</v>
       </c>
-      <c r="AT4" t="s">
+      <c r="AV4" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="5" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>211</v>
       </c>
@@ -2155,14 +2194,20 @@
       <c r="AR5" s="32">
         <v>0</v>
       </c>
-      <c r="AS5" t="s">
+      <c r="AS5" s="32">
+        <v>0</v>
+      </c>
+      <c r="AT5" s="32">
+        <v>0</v>
+      </c>
+      <c r="AU5" t="s">
         <v>217</v>
       </c>
-      <c r="AT5" t="s">
+      <c r="AV5" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="6" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>23</v>
       </c>
@@ -2296,14 +2341,20 @@
       <c r="AR6" s="32">
         <v>0</v>
       </c>
-      <c r="AS6" t="s">
+      <c r="AS6" s="32">
+        <v>0</v>
+      </c>
+      <c r="AT6" s="32">
+        <v>0</v>
+      </c>
+      <c r="AU6" t="s">
         <v>187</v>
       </c>
-      <c r="AT6" t="s">
+      <c r="AV6" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="7" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>24</v>
       </c>
@@ -2437,14 +2488,20 @@
       <c r="AR7" s="32">
         <v>0</v>
       </c>
-      <c r="AS7" t="s">
+      <c r="AS7" s="32">
+        <v>0</v>
+      </c>
+      <c r="AT7" s="32">
+        <v>0</v>
+      </c>
+      <c r="AU7" t="s">
         <v>188</v>
       </c>
-      <c r="AT7" t="s">
+      <c r="AV7" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>39</v>
       </c>
@@ -2578,14 +2635,20 @@
       <c r="AR8" s="32">
         <v>0</v>
       </c>
-      <c r="AS8" t="s">
+      <c r="AS8" s="32">
+        <v>0</v>
+      </c>
+      <c r="AT8" s="32">
+        <v>0</v>
+      </c>
+      <c r="AU8" t="s">
         <v>194</v>
       </c>
-      <c r="AT8" t="s">
+      <c r="AV8" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="9" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>27</v>
       </c>
@@ -2719,14 +2782,20 @@
       <c r="AR9" s="32">
         <v>0</v>
       </c>
-      <c r="AS9" t="s">
+      <c r="AS9" s="32">
+        <v>0</v>
+      </c>
+      <c r="AT9" s="32">
+        <v>0</v>
+      </c>
+      <c r="AU9" t="s">
         <v>176</v>
       </c>
-      <c r="AT9" t="s">
+      <c r="AV9" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="10" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>28</v>
       </c>
@@ -2860,14 +2929,20 @@
       <c r="AR10" s="32">
         <v>0</v>
       </c>
-      <c r="AS10" t="s">
+      <c r="AS10" s="32">
+        <v>0</v>
+      </c>
+      <c r="AT10" s="32">
+        <v>0</v>
+      </c>
+      <c r="AU10" t="s">
         <v>177</v>
       </c>
-      <c r="AT10" t="s">
+      <c r="AV10" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="11" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>12</v>
       </c>
@@ -3001,14 +3076,20 @@
       <c r="AR11" s="32">
         <v>0</v>
       </c>
-      <c r="AS11" t="s">
+      <c r="AS11" s="32">
+        <v>0</v>
+      </c>
+      <c r="AT11" s="32">
+        <v>0</v>
+      </c>
+      <c r="AU11" t="s">
         <v>201</v>
       </c>
-      <c r="AT11" t="s">
+      <c r="AV11" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="12" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>29</v>
       </c>
@@ -3142,14 +3223,20 @@
       <c r="AR12" s="32">
         <v>0</v>
       </c>
-      <c r="AS12" t="s">
+      <c r="AS12" s="32">
+        <v>0</v>
+      </c>
+      <c r="AT12" s="32">
+        <v>0</v>
+      </c>
+      <c r="AU12" t="s">
         <v>202</v>
       </c>
-      <c r="AT12" t="s">
+      <c r="AV12" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="13" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>18</v>
       </c>
@@ -3283,14 +3370,20 @@
       <c r="AR13" s="32">
         <v>0</v>
       </c>
-      <c r="AS13" t="s">
+      <c r="AS13" s="32">
+        <v>0</v>
+      </c>
+      <c r="AT13" s="32">
+        <v>0</v>
+      </c>
+      <c r="AU13" t="s">
         <v>52</v>
       </c>
-      <c r="AT13" t="s">
+      <c r="AV13" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="14" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>31</v>
       </c>
@@ -3424,14 +3517,20 @@
       <c r="AR14" s="32">
         <v>0</v>
       </c>
-      <c r="AS14" t="s">
+      <c r="AS14" s="32">
+        <v>0</v>
+      </c>
+      <c r="AT14" s="32">
+        <v>0</v>
+      </c>
+      <c r="AU14" t="s">
         <v>199</v>
       </c>
-      <c r="AT14" t="s">
+      <c r="AV14" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="15" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>40</v>
       </c>
@@ -3565,14 +3664,20 @@
       <c r="AR15" s="32">
         <v>0</v>
       </c>
-      <c r="AS15" t="s">
+      <c r="AS15" s="32">
+        <v>0</v>
+      </c>
+      <c r="AT15" s="32">
+        <v>0</v>
+      </c>
+      <c r="AU15" t="s">
         <v>200</v>
       </c>
-      <c r="AT15" t="s">
+      <c r="AV15" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="16" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>32</v>
       </c>
@@ -3706,14 +3811,20 @@
       <c r="AR16" s="32">
         <v>0</v>
       </c>
-      <c r="AS16" t="s">
+      <c r="AS16" s="32">
+        <v>0</v>
+      </c>
+      <c r="AT16" s="32">
+        <v>0</v>
+      </c>
+      <c r="AU16" t="s">
         <v>191</v>
       </c>
-      <c r="AT16" t="s">
+      <c r="AV16" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="17" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>33</v>
       </c>
@@ -3847,14 +3958,20 @@
       <c r="AR17" s="32">
         <v>0</v>
       </c>
-      <c r="AS17" t="s">
+      <c r="AS17" s="32">
+        <v>0</v>
+      </c>
+      <c r="AT17" s="32">
+        <v>0</v>
+      </c>
+      <c r="AU17" t="s">
         <v>192</v>
       </c>
-      <c r="AT17" t="s">
+      <c r="AV17" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="18" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>13</v>
       </c>
@@ -3988,14 +4105,20 @@
       <c r="AR18" s="32">
         <v>0</v>
       </c>
-      <c r="AS18" t="s">
+      <c r="AS18" s="32">
+        <v>0</v>
+      </c>
+      <c r="AT18" s="32">
+        <v>0</v>
+      </c>
+      <c r="AU18" t="s">
         <v>193</v>
       </c>
-      <c r="AT18" t="s">
+      <c r="AV18" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="19" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>34</v>
       </c>
@@ -4129,14 +4252,20 @@
       <c r="AR19" s="32">
         <v>0</v>
       </c>
-      <c r="AS19" t="s">
+      <c r="AS19" s="32">
+        <v>0</v>
+      </c>
+      <c r="AT19" s="32">
+        <v>0</v>
+      </c>
+      <c r="AU19" t="s">
         <v>184</v>
       </c>
-      <c r="AT19" t="s">
+      <c r="AV19" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="20" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>35</v>
       </c>
@@ -4270,14 +4399,20 @@
       <c r="AR20" s="32">
         <v>0</v>
       </c>
-      <c r="AS20" t="s">
+      <c r="AS20" s="32">
+        <v>0</v>
+      </c>
+      <c r="AT20" s="32">
+        <v>0</v>
+      </c>
+      <c r="AU20" t="s">
         <v>180</v>
       </c>
-      <c r="AT20" t="s">
+      <c r="AV20" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="21" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>36</v>
       </c>
@@ -4411,14 +4546,20 @@
       <c r="AR21" s="32">
         <v>0</v>
       </c>
-      <c r="AS21" t="s">
+      <c r="AS21" s="32">
+        <v>0</v>
+      </c>
+      <c r="AT21" s="32">
+        <v>0</v>
+      </c>
+      <c r="AU21" t="s">
         <v>189</v>
       </c>
-      <c r="AT21" t="s">
+      <c r="AV21" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="22" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>37</v>
       </c>
@@ -4552,14 +4693,20 @@
       <c r="AR22" s="32">
         <v>0</v>
       </c>
-      <c r="AS22" t="s">
+      <c r="AS22" s="32">
+        <v>0</v>
+      </c>
+      <c r="AT22" s="32">
+        <v>0</v>
+      </c>
+      <c r="AU22" t="s">
         <v>185</v>
       </c>
-      <c r="AT22" t="s">
+      <c r="AV22" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="23" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>38</v>
       </c>
@@ -4693,14 +4840,20 @@
       <c r="AR23" s="32">
         <v>0</v>
       </c>
-      <c r="AS23" t="s">
+      <c r="AS23" s="32">
+        <v>0</v>
+      </c>
+      <c r="AT23" s="32">
+        <v>0</v>
+      </c>
+      <c r="AU23" t="s">
         <v>178</v>
       </c>
-      <c r="AT23" t="s">
+      <c r="AV23" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="24" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>30</v>
       </c>
@@ -4834,14 +4987,20 @@
       <c r="AR24" s="32">
         <v>0</v>
       </c>
-      <c r="AS24" t="s">
+      <c r="AS24" s="32">
+        <v>0</v>
+      </c>
+      <c r="AT24" s="32">
+        <v>0</v>
+      </c>
+      <c r="AU24" t="s">
         <v>54</v>
       </c>
-      <c r="AT24" t="s">
+      <c r="AV24" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="25" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
         <v>207</v>
       </c>
@@ -4975,14 +5134,20 @@
       <c r="AR25" s="32">
         <v>0</v>
       </c>
-      <c r="AS25" t="s">
+      <c r="AS25" s="32">
+        <v>0</v>
+      </c>
+      <c r="AT25" s="32">
+        <v>0</v>
+      </c>
+      <c r="AU25" t="s">
         <v>207</v>
       </c>
-      <c r="AT25" t="s">
+      <c r="AV25" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="26" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
         <v>208</v>
       </c>
@@ -5116,14 +5281,20 @@
       <c r="AR26" s="32">
         <v>0</v>
       </c>
-      <c r="AS26" t="s">
+      <c r="AS26" s="32">
+        <v>0</v>
+      </c>
+      <c r="AT26" s="32">
+        <v>0</v>
+      </c>
+      <c r="AU26" t="s">
         <v>208</v>
       </c>
-      <c r="AT26" t="s">
+      <c r="AV26" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="27" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>41</v>
       </c>
@@ -5257,14 +5428,20 @@
       <c r="AR27" s="32">
         <v>0</v>
       </c>
-      <c r="AS27" t="s">
+      <c r="AS27" s="32">
+        <v>0</v>
+      </c>
+      <c r="AT27" s="32">
+        <v>0</v>
+      </c>
+      <c r="AU27" t="s">
         <v>181</v>
       </c>
-      <c r="AT27" t="s">
+      <c r="AV27" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="28" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>214</v>
       </c>
@@ -5398,14 +5575,20 @@
       <c r="AR28" s="32">
         <v>0</v>
       </c>
-      <c r="AS28" t="s">
+      <c r="AS28" s="32">
+        <v>0</v>
+      </c>
+      <c r="AT28" s="32">
+        <v>0</v>
+      </c>
+      <c r="AU28" t="s">
         <v>218</v>
       </c>
-      <c r="AT28" t="s">
+      <c r="AV28" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="29" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>42</v>
       </c>
@@ -5539,14 +5722,20 @@
       <c r="AR29" s="32">
         <v>0</v>
       </c>
-      <c r="AS29" t="s">
+      <c r="AS29" s="32">
+        <v>0</v>
+      </c>
+      <c r="AT29" s="32">
+        <v>0</v>
+      </c>
+      <c r="AU29" t="s">
         <v>219</v>
       </c>
-      <c r="AT29" t="s">
+      <c r="AV29" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="30" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>43</v>
       </c>
@@ -5680,14 +5869,20 @@
       <c r="AR30" s="32">
         <v>0</v>
       </c>
-      <c r="AS30" t="s">
+      <c r="AS30" s="32">
+        <v>0</v>
+      </c>
+      <c r="AT30" s="32">
+        <v>0</v>
+      </c>
+      <c r="AU30" t="s">
         <v>186</v>
       </c>
-      <c r="AT30" t="s">
+      <c r="AV30" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="31" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>44</v>
       </c>
@@ -5821,14 +6016,20 @@
       <c r="AR31" s="32">
         <v>0</v>
       </c>
-      <c r="AS31" t="s">
+      <c r="AS31" s="32">
+        <v>0</v>
+      </c>
+      <c r="AT31" s="32">
+        <v>0</v>
+      </c>
+      <c r="AU31" t="s">
         <v>182</v>
       </c>
-      <c r="AT31" t="s">
+      <c r="AV31" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="32" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>45</v>
       </c>
@@ -5962,14 +6163,20 @@
       <c r="AR32" s="32">
         <v>0</v>
       </c>
-      <c r="AS32" t="s">
+      <c r="AS32" s="32">
+        <v>0</v>
+      </c>
+      <c r="AT32" s="32">
+        <v>0</v>
+      </c>
+      <c r="AU32" t="s">
         <v>179</v>
       </c>
-      <c r="AT32" t="s">
+      <c r="AV32" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="33" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
         <v>15</v>
       </c>
@@ -6103,14 +6310,20 @@
       <c r="AR33" s="32">
         <v>0</v>
       </c>
-      <c r="AS33" t="s">
+      <c r="AS33" s="32">
+        <v>0</v>
+      </c>
+      <c r="AT33" s="32">
+        <v>0</v>
+      </c>
+      <c r="AU33" t="s">
         <v>195</v>
       </c>
-      <c r="AT33" t="s">
+      <c r="AV33" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="34" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
         <v>93</v>
       </c>
@@ -6244,14 +6457,20 @@
       <c r="AR34" s="32">
         <v>0</v>
       </c>
-      <c r="AS34" t="s">
+      <c r="AS34" s="32">
+        <v>0</v>
+      </c>
+      <c r="AT34" s="32">
+        <v>0</v>
+      </c>
+      <c r="AU34" t="s">
         <v>92</v>
       </c>
-      <c r="AT34" t="s">
+      <c r="AV34" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="35" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>46</v>
       </c>
@@ -6385,14 +6604,20 @@
       <c r="AR35" s="32">
         <v>0</v>
       </c>
-      <c r="AS35" t="s">
+      <c r="AS35" s="32">
+        <v>0</v>
+      </c>
+      <c r="AT35" s="32">
+        <v>0</v>
+      </c>
+      <c r="AU35" t="s">
         <v>183</v>
       </c>
-      <c r="AT35" t="s">
+      <c r="AV35" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="36" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>205</v>
       </c>
@@ -6526,14 +6751,20 @@
       <c r="AR36" s="32">
         <v>0</v>
       </c>
-      <c r="AS36" t="s">
+      <c r="AS36" s="32">
+        <v>0</v>
+      </c>
+      <c r="AT36" s="32">
+        <v>0</v>
+      </c>
+      <c r="AU36" t="s">
         <v>205</v>
       </c>
-      <c r="AT36" t="s">
+      <c r="AV36" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="37" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>209</v>
       </c>
@@ -6667,14 +6898,20 @@
       <c r="AR37" s="32">
         <v>0</v>
       </c>
-      <c r="AS37" t="s">
+      <c r="AS37" s="32">
+        <v>0</v>
+      </c>
+      <c r="AT37" s="32">
+        <v>0</v>
+      </c>
+      <c r="AU37" t="s">
         <v>216</v>
       </c>
-      <c r="AT37" t="s">
+      <c r="AV37" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="38" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>47</v>
       </c>
@@ -6808,14 +7045,20 @@
       <c r="AR38" s="32">
         <v>0</v>
       </c>
-      <c r="AS38" t="s">
+      <c r="AS38" s="32">
+        <v>0</v>
+      </c>
+      <c r="AT38" s="32">
+        <v>0</v>
+      </c>
+      <c r="AU38" t="s">
         <v>190</v>
       </c>
-      <c r="AT38" t="s">
+      <c r="AV38" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="39" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
         <v>245</v>
       </c>
@@ -6949,11 +7192,17 @@
       <c r="AR39" s="32">
         <v>0</v>
       </c>
-      <c r="AS39" t="s">
+      <c r="AS39" s="32">
+        <v>0</v>
+      </c>
+      <c r="AT39" s="32">
+        <v>0</v>
+      </c>
+      <c r="AU39" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="40" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A40" s="13" t="s">
         <v>258</v>
       </c>
@@ -7086,14 +7335,20 @@
       <c r="AR40" s="32">
         <v>1</v>
       </c>
-      <c r="AS40" t="s">
+      <c r="AS40" s="32">
+        <v>1</v>
+      </c>
+      <c r="AT40" s="32">
+        <v>1</v>
+      </c>
+      <c r="AU40" t="s">
         <v>260</v>
       </c>
-      <c r="AT40" t="s">
+      <c r="AV40" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="42" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:48" x14ac:dyDescent="0.25">
       <c r="AF42" t="s">
         <v>204</v>
       </c>
@@ -7105,10 +7360,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:EM40"/>
+  <dimension ref="A1:ER40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="T1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="EE38" sqref="EE38"/>
+    <sheetView tabSelected="1" topLeftCell="AA1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AR50" sqref="AR50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7116,11 +7371,11 @@
     <col min="1" max="75" width="3.7109375" bestFit="1" customWidth="1"/>
     <col min="76" max="77" width="3.7109375" customWidth="1"/>
     <col min="78" max="86" width="3.7109375" bestFit="1" customWidth="1"/>
-    <col min="87" max="142" width="3.7109375" customWidth="1"/>
-    <col min="143" max="143" width="36.28515625" customWidth="1"/>
+    <col min="87" max="147" width="3.7109375" customWidth="1"/>
+    <col min="148" max="148" width="36.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:143" s="11" customFormat="1" ht="72" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:148" s="11" customFormat="1" ht="72" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>95</v>
       </c>
@@ -7545,13 +7800,28 @@
         <v>297</v>
       </c>
       <c r="EL1" s="11" t="s">
+        <v>298</v>
+      </c>
+      <c r="EM1" s="11" t="s">
+        <v>299</v>
+      </c>
+      <c r="EN1" s="11" t="s">
+        <v>300</v>
+      </c>
+      <c r="EO1" s="11" t="s">
+        <v>301</v>
+      </c>
+      <c r="EP1" s="11" t="s">
+        <v>302</v>
+      </c>
+      <c r="EQ1" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="EM1" t="s">
+      <c r="ER1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:143" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:148" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>88</v>
       </c>
@@ -8010,15 +8280,32 @@
       <c r="EK2" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="EL2" s="12" t="s">
+      <c r="EL2" s="12">
+        <f>Tabelle1!AS2</f>
+        <v>0</v>
+      </c>
+      <c r="EM2" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EN2" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EO2" s="12">
+        <f>Tabelle1!AT2</f>
+        <v>0</v>
+      </c>
+      <c r="EP2" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EQ2" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EM2" t="str">
-        <f>Tabelle1!AS2</f>
+      <c r="ER2" t="str">
+        <f>Tabelle1!AU2</f>
         <v>Airbus A320 Neo</v>
       </c>
     </row>
-    <row r="3" spans="1:143" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:148" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
         <v>88</v>
       </c>
@@ -8477,15 +8764,32 @@
       <c r="EK3" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="EL3" s="12" t="s">
+      <c r="EL3" s="12">
+        <f>Tabelle1!AS3</f>
+        <v>0</v>
+      </c>
+      <c r="EM3" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EN3" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EO3" s="12">
+        <f>Tabelle1!AT3</f>
+        <v>0</v>
+      </c>
+      <c r="EP3" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EQ3" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EM3" t="str">
-        <f>Tabelle1!AS3</f>
+      <c r="ER3" t="str">
+        <f>Tabelle1!AU3</f>
         <v>Boeing 747-8i</v>
       </c>
     </row>
-    <row r="4" spans="1:143" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:148" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
         <v>88</v>
       </c>
@@ -8944,15 +9248,32 @@
       <c r="EK4" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="EL4" s="12" t="s">
+      <c r="EL4" s="12">
+        <f>Tabelle1!AS4</f>
+        <v>0</v>
+      </c>
+      <c r="EM4" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EN4" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EO4" s="12">
+        <f>Tabelle1!AT4</f>
+        <v>0</v>
+      </c>
+      <c r="EP4" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EQ4" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EM4" t="str">
-        <f>Tabelle1!AS4</f>
+      <c r="ER4" t="str">
+        <f>Tabelle1!AU4</f>
         <v>Boeing 787-10</v>
       </c>
     </row>
-    <row r="5" spans="1:143" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:148" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>88</v>
       </c>
@@ -9411,15 +9732,32 @@
       <c r="EK5" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="EL5" s="12" t="s">
+      <c r="EL5" s="12">
+        <f>Tabelle1!AS5</f>
+        <v>0</v>
+      </c>
+      <c r="EM5" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EN5" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EO5" s="12">
+        <f>Tabelle1!AT5</f>
+        <v>0</v>
+      </c>
+      <c r="EP5" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EQ5" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EM5" t="str">
-        <f>Tabelle1!AS5</f>
+      <c r="ER5" t="str">
+        <f>Tabelle1!AU5</f>
         <v>Boeing F/A 18E Super Hornet</v>
       </c>
     </row>
-    <row r="6" spans="1:143" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:148" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>88</v>
       </c>
@@ -9878,15 +10216,32 @@
       <c r="EK6" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="EL6" s="12" t="s">
+      <c r="EL6" s="12">
+        <f>Tabelle1!AS6</f>
+        <v>0</v>
+      </c>
+      <c r="EM6" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EN6" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EO6" s="12">
+        <f>Tabelle1!AT6</f>
+        <v>0</v>
+      </c>
+      <c r="EP6" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EQ6" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EM6" t="str">
-        <f>Tabelle1!AS6</f>
+      <c r="ER6" t="str">
+        <f>Tabelle1!AU6</f>
         <v>Baron G58</v>
       </c>
     </row>
-    <row r="7" spans="1:143" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:148" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>88</v>
       </c>
@@ -10345,15 +10700,32 @@
       <c r="EK7" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="EL7" s="12" t="s">
+      <c r="EL7" s="12">
+        <f>Tabelle1!AS7</f>
+        <v>0</v>
+      </c>
+      <c r="EM7" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EN7" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EO7" s="12">
+        <f>Tabelle1!AT7</f>
+        <v>0</v>
+      </c>
+      <c r="EP7" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EQ7" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EM7" t="str">
-        <f>Tabelle1!AS7</f>
+      <c r="ER7" t="str">
+        <f>Tabelle1!AU7</f>
         <v>Bonanza G36</v>
       </c>
     </row>
-    <row r="8" spans="1:143" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:148" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>88</v>
       </c>
@@ -10812,15 +11184,32 @@
       <c r="EK8" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="EL8" s="12" t="s">
+      <c r="EL8" s="12">
+        <f>Tabelle1!AS8</f>
+        <v>0</v>
+      </c>
+      <c r="EM8" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EN8" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EO8" s="12">
+        <f>Tabelle1!AT8</f>
+        <v>0</v>
+      </c>
+      <c r="EP8" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EQ8" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EM8" t="str">
-        <f>Tabelle1!AS8</f>
+      <c r="ER8" t="str">
+        <f>Tabelle1!AU8</f>
         <v>Beechcraft King Air 350i</v>
       </c>
     </row>
-    <row r="9" spans="1:143" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:148" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>88</v>
       </c>
@@ -11279,15 +11668,32 @@
       <c r="EK9" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="EL9" s="12" t="s">
+      <c r="EL9" s="12">
+        <f>Tabelle1!AS9</f>
+        <v>0</v>
+      </c>
+      <c r="EM9" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EN9" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EO9" s="12">
+        <f>Tabelle1!AT9</f>
+        <v>0</v>
+      </c>
+      <c r="EP9" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EQ9" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EM9" t="str">
-        <f>Tabelle1!AS9</f>
+      <c r="ER9" t="str">
+        <f>Tabelle1!AU9</f>
         <v>Cessna 152</v>
       </c>
     </row>
-    <row r="10" spans="1:143" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:148" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
         <v>88</v>
       </c>
@@ -11746,15 +12152,32 @@
       <c r="EK10" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="EL10" s="12" t="s">
+      <c r="EL10" s="12">
+        <f>Tabelle1!AS10</f>
+        <v>0</v>
+      </c>
+      <c r="EM10" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EN10" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EO10" s="12">
+        <f>Tabelle1!AT10</f>
+        <v>0</v>
+      </c>
+      <c r="EP10" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EQ10" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EM10" t="str">
-        <f>Tabelle1!AS10</f>
+      <c r="ER10" t="str">
+        <f>Tabelle1!AU10</f>
         <v>Cessna 152 Aero</v>
       </c>
     </row>
-    <row r="11" spans="1:143" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:148" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
         <v>88</v>
       </c>
@@ -12213,15 +12636,32 @@
       <c r="EK11" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="EL11" s="12" t="s">
+      <c r="EL11" s="12">
+        <f>Tabelle1!AS11</f>
+        <v>0</v>
+      </c>
+      <c r="EM11" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EN11" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EO11" s="12">
+        <f>Tabelle1!AT11</f>
+        <v>0</v>
+      </c>
+      <c r="EP11" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EQ11" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EM11" t="str">
-        <f>Tabelle1!AS11</f>
+      <c r="ER11" t="str">
+        <f>Tabelle1!AU11</f>
         <v>Cessna 172sp Skyhawk G1000</v>
       </c>
     </row>
-    <row r="12" spans="1:143" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:148" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
         <v>88</v>
       </c>
@@ -12680,15 +13120,32 @@
       <c r="EK12" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="EL12" s="12" t="s">
+      <c r="EL12" s="12">
+        <f>Tabelle1!AS12</f>
+        <v>0</v>
+      </c>
+      <c r="EM12" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EN12" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EO12" s="12">
+        <f>Tabelle1!AT12</f>
+        <v>0</v>
+      </c>
+      <c r="EP12" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EQ12" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EM12" t="str">
-        <f>Tabelle1!AS12</f>
+      <c r="ER12" t="str">
+        <f>Tabelle1!AU12</f>
         <v>Cessna 172sp Skyhawk</v>
       </c>
     </row>
-    <row r="13" spans="1:143" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:148" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
         <v>88</v>
       </c>
@@ -13147,15 +13604,32 @@
       <c r="EK13" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="EL13" s="12" t="s">
+      <c r="EL13" s="12">
+        <f>Tabelle1!AS13</f>
+        <v>0</v>
+      </c>
+      <c r="EM13" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EN13" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EO13" s="12">
+        <f>Tabelle1!AT13</f>
+        <v>0</v>
+      </c>
+      <c r="EP13" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EQ13" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EM13" t="str">
-        <f>Tabelle1!AS13</f>
+      <c r="ER13" t="str">
+        <f>Tabelle1!AU13</f>
         <v>Cessna 208B Grand Caravan EX</v>
       </c>
     </row>
-    <row r="14" spans="1:143" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:148" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
         <v>88</v>
       </c>
@@ -13614,15 +14088,32 @@
       <c r="EK14" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="EL14" s="12" t="s">
+      <c r="EL14" s="12">
+        <f>Tabelle1!AS14</f>
+        <v>0</v>
+      </c>
+      <c r="EM14" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EN14" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EO14" s="12">
+        <f>Tabelle1!AT14</f>
+        <v>0</v>
+      </c>
+      <c r="EP14" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EQ14" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EM14" t="str">
-        <f>Tabelle1!AS14</f>
+      <c r="ER14" t="str">
+        <f>Tabelle1!AU14</f>
         <v>Cessna CJ4 Citation</v>
       </c>
     </row>
-    <row r="15" spans="1:143" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:148" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
         <v>88</v>
       </c>
@@ -14081,15 +14572,32 @@
       <c r="EK15" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="EL15" s="12" t="s">
+      <c r="EL15" s="12">
+        <f>Tabelle1!AS15</f>
+        <v>0</v>
+      </c>
+      <c r="EM15" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EN15" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EO15" s="12">
+        <f>Tabelle1!AT15</f>
+        <v>0</v>
+      </c>
+      <c r="EP15" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EQ15" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EM15" t="str">
-        <f>Tabelle1!AS15</f>
+      <c r="ER15" t="str">
+        <f>Tabelle1!AU15</f>
         <v>Cessna Longitude</v>
       </c>
     </row>
-    <row r="16" spans="1:143" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:148" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
         <v>88</v>
       </c>
@@ -14548,15 +15056,32 @@
       <c r="EK16" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="EL16" s="12" t="s">
+      <c r="EL16" s="12">
+        <f>Tabelle1!AS16</f>
+        <v>0</v>
+      </c>
+      <c r="EM16" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EN16" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EO16" s="12">
+        <f>Tabelle1!AT16</f>
+        <v>0</v>
+      </c>
+      <c r="EP16" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EQ16" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EM16" t="str">
-        <f>Tabelle1!AS16</f>
+      <c r="ER16" t="str">
+        <f>Tabelle1!AU16</f>
         <v>DA40-NG</v>
       </c>
     </row>
-    <row r="17" spans="1:143" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:148" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
         <v>88</v>
       </c>
@@ -15015,15 +15540,32 @@
       <c r="EK17" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="EL17" s="12" t="s">
+      <c r="EL17" s="12">
+        <f>Tabelle1!AS17</f>
+        <v>0</v>
+      </c>
+      <c r="EM17" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EN17" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EO17" s="12">
+        <f>Tabelle1!AT17</f>
+        <v>0</v>
+      </c>
+      <c r="EP17" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EQ17" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EM17" t="str">
-        <f>Tabelle1!AS17</f>
+      <c r="ER17" t="str">
+        <f>Tabelle1!AU17</f>
         <v>DA40 TDI</v>
       </c>
     </row>
-    <row r="18" spans="1:143" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:148" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
         <v>88</v>
       </c>
@@ -15482,15 +16024,32 @@
       <c r="EK18" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="EL18" s="12" t="s">
+      <c r="EL18" s="12">
+        <f>Tabelle1!AS18</f>
+        <v>0</v>
+      </c>
+      <c r="EM18" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EN18" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EO18" s="12">
+        <f>Tabelle1!AT18</f>
+        <v>0</v>
+      </c>
+      <c r="EP18" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EQ18" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EM18" t="str">
-        <f>Tabelle1!AS18</f>
+      <c r="ER18" t="str">
+        <f>Tabelle1!AU18</f>
         <v>DA62</v>
       </c>
     </row>
-    <row r="19" spans="1:143" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:148" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
         <v>88</v>
       </c>
@@ -15949,15 +16508,32 @@
       <c r="EK19" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="EL19" s="12" t="s">
+      <c r="EL19" s="12">
+        <f>Tabelle1!AS19</f>
+        <v>0</v>
+      </c>
+      <c r="EM19" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EN19" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EO19" s="12">
+        <f>Tabelle1!AT19</f>
+        <v>0</v>
+      </c>
+      <c r="EP19" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EQ19" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EM19" t="str">
-        <f>Tabelle1!AS19</f>
+      <c r="ER19" t="str">
+        <f>Tabelle1!AU19</f>
         <v>DR400</v>
       </c>
     </row>
-    <row r="20" spans="1:143" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:148" x14ac:dyDescent="0.25">
       <c r="A20" s="12" t="s">
         <v>88</v>
       </c>
@@ -16416,15 +16992,32 @@
       <c r="EK20" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="EL20" s="12" t="s">
+      <c r="EL20" s="12">
+        <f>Tabelle1!AS20</f>
+        <v>0</v>
+      </c>
+      <c r="EM20" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EN20" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EO20" s="12">
+        <f>Tabelle1!AT20</f>
+        <v>0</v>
+      </c>
+      <c r="EP20" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EQ20" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EM20" t="str">
-        <f>Tabelle1!AS20</f>
+      <c r="ER20" t="str">
+        <f>Tabelle1!AU20</f>
         <v>DV20</v>
       </c>
     </row>
-    <row r="21" spans="1:143" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:148" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
         <v>88</v>
       </c>
@@ -16883,15 +17476,32 @@
       <c r="EK21" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="EL21" s="12" t="s">
+      <c r="EL21" s="12">
+        <f>Tabelle1!AS21</f>
+        <v>0</v>
+      </c>
+      <c r="EM21" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EN21" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EO21" s="12">
+        <f>Tabelle1!AT21</f>
+        <v>0</v>
+      </c>
+      <c r="EP21" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EQ21" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EM21" t="str">
-        <f>Tabelle1!AS21</f>
+      <c r="ER21" t="str">
+        <f>Tabelle1!AU21</f>
         <v>Extra 330</v>
       </c>
     </row>
-    <row r="22" spans="1:143" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:148" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="s">
         <v>88</v>
       </c>
@@ -17350,15 +17960,32 @@
       <c r="EK22" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="EL22" s="12" t="s">
+      <c r="EL22" s="12">
+        <f>Tabelle1!AS22</f>
+        <v>0</v>
+      </c>
+      <c r="EM22" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EN22" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EO22" s="12">
+        <f>Tabelle1!AT22</f>
+        <v>0</v>
+      </c>
+      <c r="EP22" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EQ22" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EM22" t="str">
-        <f>Tabelle1!AS22</f>
+      <c r="ER22" t="str">
+        <f>Tabelle1!AU22</f>
         <v>FlightDesignCT</v>
       </c>
     </row>
-    <row r="23" spans="1:143" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:148" x14ac:dyDescent="0.25">
       <c r="A23" s="12" t="s">
         <v>88</v>
       </c>
@@ -17817,15 +18444,32 @@
       <c r="EK23" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="EL23" s="12" t="s">
+      <c r="EL23" s="12">
+        <f>Tabelle1!AS23</f>
+        <v>0</v>
+      </c>
+      <c r="EM23" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EN23" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EO23" s="12">
+        <f>Tabelle1!AT23</f>
+        <v>0</v>
+      </c>
+      <c r="EP23" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EQ23" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EM23" t="str">
-        <f>Tabelle1!AS23</f>
+      <c r="ER23" t="str">
+        <f>Tabelle1!AU23</f>
         <v>Icon A5</v>
       </c>
     </row>
-    <row r="24" spans="1:143" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:148" x14ac:dyDescent="0.25">
       <c r="A24" s="12" t="s">
         <v>88</v>
       </c>
@@ -18284,15 +18928,32 @@
       <c r="EK24" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="EL24" s="12" t="s">
+      <c r="EL24" s="12">
+        <f>Tabelle1!AS24</f>
+        <v>0</v>
+      </c>
+      <c r="EM24" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EN24" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EO24" s="12">
+        <f>Tabelle1!AT24</f>
+        <v>0</v>
+      </c>
+      <c r="EP24" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EQ24" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EM24" t="str">
-        <f>Tabelle1!AS24</f>
+      <c r="ER24" t="str">
+        <f>Tabelle1!AU24</f>
         <v>Mudry Cap 10 C</v>
       </c>
     </row>
-    <row r="25" spans="1:143" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:148" x14ac:dyDescent="0.25">
       <c r="A25" s="12" t="s">
         <v>88</v>
       </c>
@@ -18751,15 +19412,32 @@
       <c r="EK25" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="EL25" s="12" t="s">
+      <c r="EL25" s="12">
+        <f>Tabelle1!AS25</f>
+        <v>0</v>
+      </c>
+      <c r="EM25" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EN25" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EO25" s="12">
+        <f>Tabelle1!AT25</f>
+        <v>0</v>
+      </c>
+      <c r="EP25" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EQ25" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EM25" t="str">
-        <f>Tabelle1!AS25</f>
+      <c r="ER25" t="str">
+        <f>Tabelle1!AU25</f>
         <v>Pilatus PC-6 Gauge</v>
       </c>
     </row>
-    <row r="26" spans="1:143" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:148" x14ac:dyDescent="0.25">
       <c r="A26" s="12" t="s">
         <v>88</v>
       </c>
@@ -19218,15 +19896,32 @@
       <c r="EK26" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="EL26" s="12" t="s">
+      <c r="EL26" s="12">
+        <f>Tabelle1!AS26</f>
+        <v>0</v>
+      </c>
+      <c r="EM26" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EN26" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EO26" s="12">
+        <f>Tabelle1!AT26</f>
+        <v>0</v>
+      </c>
+      <c r="EP26" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EQ26" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EM26" t="str">
-        <f>Tabelle1!AS26</f>
+      <c r="ER26" t="str">
+        <f>Tabelle1!AU26</f>
         <v>Pilatus PC-6 G950</v>
       </c>
     </row>
-    <row r="27" spans="1:143" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:148" x14ac:dyDescent="0.25">
       <c r="A27" s="12" t="s">
         <v>88</v>
       </c>
@@ -19685,15 +20380,32 @@
       <c r="EK27" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="EL27" s="12" t="s">
+      <c r="EL27" s="12">
+        <f>Tabelle1!AS27</f>
+        <v>0</v>
+      </c>
+      <c r="EM27" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EN27" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EO27" s="12">
+        <f>Tabelle1!AT27</f>
+        <v>0</v>
+      </c>
+      <c r="EP27" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EQ27" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EM27" t="str">
-        <f>Tabelle1!AS27</f>
+      <c r="ER27" t="str">
+        <f>Tabelle1!AU27</f>
         <v>Pipistrel Alpha Electro</v>
       </c>
     </row>
-    <row r="28" spans="1:143" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:148" x14ac:dyDescent="0.25">
       <c r="A28" s="12" t="s">
         <v>88</v>
       </c>
@@ -20152,15 +20864,32 @@
       <c r="EK28" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="EL28" s="12" t="s">
+      <c r="EL28" s="12">
+        <f>Tabelle1!AS28</f>
+        <v>0</v>
+      </c>
+      <c r="EM28" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EN28" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EO28" s="12">
+        <f>Tabelle1!AT28</f>
+        <v>0</v>
+      </c>
+      <c r="EP28" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EQ28" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EM28" t="str">
-        <f>Tabelle1!AS28</f>
+      <c r="ER28" t="str">
+        <f>Tabelle1!AU28</f>
         <v>Pitts Special 1S</v>
       </c>
     </row>
-    <row r="29" spans="1:143" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:148" x14ac:dyDescent="0.25">
       <c r="A29" s="12" t="s">
         <v>88</v>
       </c>
@@ -20619,15 +21348,32 @@
       <c r="EK29" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="EL29" s="12" t="s">
+      <c r="EL29" s="12">
+        <f>Tabelle1!AS29</f>
+        <v>0</v>
+      </c>
+      <c r="EM29" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EN29" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EO29" s="12">
+        <f>Tabelle1!AT29</f>
+        <v>0</v>
+      </c>
+      <c r="EP29" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EQ29" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EM29" t="str">
-        <f>Tabelle1!AS29</f>
+      <c r="ER29" t="str">
+        <f>Tabelle1!AU29</f>
         <v>Pitts Special S2S</v>
       </c>
     </row>
-    <row r="30" spans="1:143" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:148" x14ac:dyDescent="0.25">
       <c r="A30" s="12" t="s">
         <v>88</v>
       </c>
@@ -21086,15 +21832,32 @@
       <c r="EK30" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="EL30" s="12" t="s">
+      <c r="EL30" s="12">
+        <f>Tabelle1!AS30</f>
+        <v>0</v>
+      </c>
+      <c r="EM30" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EN30" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EO30" s="12">
+        <f>Tabelle1!AT30</f>
+        <v>0</v>
+      </c>
+      <c r="EP30" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EQ30" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EM30" t="str">
-        <f>Tabelle1!AS30</f>
+      <c r="ER30" t="str">
+        <f>Tabelle1!AU30</f>
         <v>Savage Cub</v>
       </c>
     </row>
-    <row r="31" spans="1:143" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:148" x14ac:dyDescent="0.25">
       <c r="A31" s="12" t="s">
         <v>88</v>
       </c>
@@ -21553,15 +22316,32 @@
       <c r="EK31" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="EL31" s="12" t="s">
+      <c r="EL31" s="12">
+        <f>Tabelle1!AS31</f>
+        <v>0</v>
+      </c>
+      <c r="EM31" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EN31" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EO31" s="12">
+        <f>Tabelle1!AT31</f>
+        <v>0</v>
+      </c>
+      <c r="EP31" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EQ31" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EM31" t="str">
-        <f>Tabelle1!AS31</f>
+      <c r="ER31" t="str">
+        <f>Tabelle1!AU31</f>
         <v>Savage Shock Ultra</v>
       </c>
     </row>
-    <row r="32" spans="1:143" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:148" x14ac:dyDescent="0.25">
       <c r="A32" s="12" t="s">
         <v>88</v>
       </c>
@@ -22020,15 +22800,32 @@
       <c r="EK32" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="EL32" s="12" t="s">
+      <c r="EL32" s="12">
+        <f>Tabelle1!AS32</f>
+        <v>0</v>
+      </c>
+      <c r="EM32" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EN32" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EO32" s="12">
+        <f>Tabelle1!AT32</f>
+        <v>0</v>
+      </c>
+      <c r="EP32" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EQ32" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EM32" t="str">
-        <f>Tabelle1!AS32</f>
+      <c r="ER32" t="str">
+        <f>Tabelle1!AU32</f>
         <v>SR22</v>
       </c>
     </row>
-    <row r="33" spans="1:143" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:148" x14ac:dyDescent="0.25">
       <c r="A33" s="12" t="s">
         <v>88</v>
       </c>
@@ -22487,15 +23284,32 @@
       <c r="EK33" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="EL33" s="12" t="s">
+      <c r="EL33" s="12">
+        <f>Tabelle1!AS33</f>
+        <v>0</v>
+      </c>
+      <c r="EM33" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EN33" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EO33" s="12">
+        <f>Tabelle1!AT33</f>
+        <v>0</v>
+      </c>
+      <c r="EP33" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EQ33" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EM33" t="str">
-        <f>Tabelle1!AS33</f>
+      <c r="ER33" t="str">
+        <f>Tabelle1!AU33</f>
         <v>TBM 930</v>
       </c>
     </row>
-    <row r="34" spans="1:143" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:148" x14ac:dyDescent="0.25">
       <c r="A34" s="12" t="s">
         <v>88</v>
       </c>
@@ -22954,15 +23768,32 @@
       <c r="EK34" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="EL34" s="12" t="s">
+      <c r="EL34" s="12">
+        <f>Tabelle1!AS34</f>
+        <v>0</v>
+      </c>
+      <c r="EM34" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EN34" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EO34" s="12">
+        <f>Tabelle1!AT34</f>
+        <v>0</v>
+      </c>
+      <c r="EP34" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EQ34" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EM34" t="str">
-        <f>Tabelle1!AS34</f>
+      <c r="ER34" t="str">
+        <f>Tabelle1!AU34</f>
         <v>Vertigo</v>
       </c>
     </row>
-    <row r="35" spans="1:143" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:148" x14ac:dyDescent="0.25">
       <c r="A35" s="12" t="s">
         <v>88</v>
       </c>
@@ -23421,15 +24252,32 @@
       <c r="EK35" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="EL35" s="12" t="s">
+      <c r="EL35" s="12">
+        <f>Tabelle1!AS35</f>
+        <v>0</v>
+      </c>
+      <c r="EM35" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EN35" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EO35" s="12">
+        <f>Tabelle1!AT35</f>
+        <v>0</v>
+      </c>
+      <c r="EP35" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EQ35" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EM35" t="str">
-        <f>Tabelle1!AS35</f>
+      <c r="ER35" t="str">
+        <f>Tabelle1!AU35</f>
         <v>VL3</v>
       </c>
     </row>
-    <row r="36" spans="1:143" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:148" x14ac:dyDescent="0.25">
       <c r="A36" s="12" t="s">
         <v>88</v>
       </c>
@@ -23888,15 +24736,32 @@
       <c r="EK36" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="EL36" s="12" t="s">
+      <c r="EL36" s="12">
+        <f>Tabelle1!AS36</f>
+        <v>0</v>
+      </c>
+      <c r="EM36" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EN36" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EO36" s="12">
+        <f>Tabelle1!AT36</f>
+        <v>0</v>
+      </c>
+      <c r="EP36" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EQ36" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EM36" t="str">
-        <f>Tabelle1!AS36</f>
+      <c r="ER36" t="str">
+        <f>Tabelle1!AU36</f>
         <v>Volocity</v>
       </c>
     </row>
-    <row r="37" spans="1:143" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:148" x14ac:dyDescent="0.25">
       <c r="A37" s="12" t="s">
         <v>88</v>
       </c>
@@ -24355,15 +25220,32 @@
       <c r="EK37" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="EL37" s="12" t="s">
+      <c r="EL37" s="12">
+        <f>Tabelle1!AS37</f>
+        <v>0</v>
+      </c>
+      <c r="EM37" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EN37" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EO37" s="12">
+        <f>Tabelle1!AT37</f>
+        <v>0</v>
+      </c>
+      <c r="EP37" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EQ37" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EM37" t="str">
-        <f>Tabelle1!AS37</f>
+      <c r="ER37" t="str">
+        <f>Tabelle1!AU37</f>
         <v>NXCub</v>
       </c>
     </row>
-    <row r="38" spans="1:143" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:148" x14ac:dyDescent="0.25">
       <c r="A38" s="12" t="s">
         <v>88</v>
       </c>
@@ -24822,15 +25704,32 @@
       <c r="EK38" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="EL38" s="12" t="s">
+      <c r="EL38" s="12">
+        <f>Tabelle1!AS38</f>
+        <v>0</v>
+      </c>
+      <c r="EM38" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EN38" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EO38" s="12">
+        <f>Tabelle1!AT38</f>
+        <v>0</v>
+      </c>
+      <c r="EP38" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EQ38" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EM38" t="str">
-        <f>Tabelle1!AS38</f>
+      <c r="ER38" t="str">
+        <f>Tabelle1!AU38</f>
         <v>XCub</v>
       </c>
     </row>
-    <row r="39" spans="1:143" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:148" x14ac:dyDescent="0.25">
       <c r="A39" s="12" t="s">
         <v>88</v>
       </c>
@@ -25289,15 +26188,32 @@
       <c r="EK39" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="EL39" s="12" t="s">
+      <c r="EL39" s="12">
+        <f>Tabelle1!AS39</f>
+        <v>0</v>
+      </c>
+      <c r="EM39" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EN39" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EO39" s="12">
+        <f>Tabelle1!AT39</f>
+        <v>0</v>
+      </c>
+      <c r="EP39" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EQ39" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EM39" t="str">
-        <f>Tabelle1!AS39</f>
+      <c r="ER39" t="str">
+        <f>Tabelle1!AU39</f>
         <v>SWS Kodiak 100 II</v>
       </c>
     </row>
-    <row r="40" spans="1:143" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:148" x14ac:dyDescent="0.25">
       <c r="A40" s="12" t="s">
         <v>88</v>
       </c>
@@ -25756,11 +26672,28 @@
       <c r="EK40" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="EL40" s="12" t="s">
+      <c r="EL40" s="12">
+        <f>Tabelle1!AS40</f>
+        <v>1</v>
+      </c>
+      <c r="EM40" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EN40" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EO40" s="12">
+        <f>Tabelle1!AT40</f>
+        <v>1</v>
+      </c>
+      <c r="EP40" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="EQ40" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="EM40" t="str">
-        <f>Tabelle1!AS40</f>
+      <c r="ER40" t="str">
+        <f>Tabelle1!AU40</f>
         <v>Generic Glider</v>
       </c>
     </row>

</xml_diff>

<commit_message>
V 0.60-B60 - final - Add PositiveRate Callout (criteria see QuickGuide) - Add Water Ballast Gauges for Gliders (quantity and flow) - Update FlightBag Map handling improved - Update DataLoader fix reading of airport names (file changed in SU11) - Update QuickGuide
</commit_message>
<xml_diff>
--- a/FS20_HudBar/Config/EngineMerge.xlsx
+++ b/FS20_HudBar/Config/EngineMerge.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4642" uniqueCount="303">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4682" uniqueCount="304">
   <si>
     <t>ACFT</t>
   </si>
@@ -927,6 +927,9 @@
   </si>
   <si>
     <t>MCRAD_KT</t>
+  </si>
+  <si>
+    <t>WBALLAST_ANI</t>
   </si>
 </sst>
 </file>
@@ -7360,10 +7363,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:ER40"/>
+  <dimension ref="A1:ES40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AA1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AR50" sqref="AR50"/>
+    <sheetView tabSelected="1" topLeftCell="BV1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="EG18" sqref="EG18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7371,11 +7374,11 @@
     <col min="1" max="75" width="3.7109375" bestFit="1" customWidth="1"/>
     <col min="76" max="77" width="3.7109375" customWidth="1"/>
     <col min="78" max="86" width="3.7109375" bestFit="1" customWidth="1"/>
-    <col min="87" max="147" width="3.7109375" customWidth="1"/>
-    <col min="148" max="148" width="36.28515625" customWidth="1"/>
+    <col min="87" max="148" width="3.7109375" customWidth="1"/>
+    <col min="149" max="149" width="36.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:148" s="11" customFormat="1" ht="72" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:149" s="11" customFormat="1" ht="75.75" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>95</v>
       </c>
@@ -7815,13 +7818,16 @@
         <v>302</v>
       </c>
       <c r="EQ1" s="11" t="s">
+        <v>303</v>
+      </c>
+      <c r="ER1" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="ER1" t="s">
+      <c r="ES1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:148" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:149" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>88</v>
       </c>
@@ -8298,14 +8304,17 @@
         <v>88</v>
       </c>
       <c r="EQ2" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="ER2" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="ER2" t="str">
+      <c r="ES2" t="str">
         <f>Tabelle1!AU2</f>
         <v>Airbus A320 Neo</v>
       </c>
     </row>
-    <row r="3" spans="1:148" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:149" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
         <v>88</v>
       </c>
@@ -8782,14 +8791,17 @@
         <v>88</v>
       </c>
       <c r="EQ3" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="ER3" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="ER3" t="str">
+      <c r="ES3" t="str">
         <f>Tabelle1!AU3</f>
         <v>Boeing 747-8i</v>
       </c>
     </row>
-    <row r="4" spans="1:148" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:149" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
         <v>88</v>
       </c>
@@ -9266,14 +9278,17 @@
         <v>88</v>
       </c>
       <c r="EQ4" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="ER4" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="ER4" t="str">
+      <c r="ES4" t="str">
         <f>Tabelle1!AU4</f>
         <v>Boeing 787-10</v>
       </c>
     </row>
-    <row r="5" spans="1:148" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:149" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>88</v>
       </c>
@@ -9750,14 +9765,17 @@
         <v>88</v>
       </c>
       <c r="EQ5" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="ER5" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="ER5" t="str">
+      <c r="ES5" t="str">
         <f>Tabelle1!AU5</f>
         <v>Boeing F/A 18E Super Hornet</v>
       </c>
     </row>
-    <row r="6" spans="1:148" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:149" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>88</v>
       </c>
@@ -10234,14 +10252,17 @@
         <v>88</v>
       </c>
       <c r="EQ6" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="ER6" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="ER6" t="str">
+      <c r="ES6" t="str">
         <f>Tabelle1!AU6</f>
         <v>Baron G58</v>
       </c>
     </row>
-    <row r="7" spans="1:148" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:149" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>88</v>
       </c>
@@ -10718,14 +10739,17 @@
         <v>88</v>
       </c>
       <c r="EQ7" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="ER7" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="ER7" t="str">
+      <c r="ES7" t="str">
         <f>Tabelle1!AU7</f>
         <v>Bonanza G36</v>
       </c>
     </row>
-    <row r="8" spans="1:148" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:149" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>88</v>
       </c>
@@ -11202,14 +11226,17 @@
         <v>88</v>
       </c>
       <c r="EQ8" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="ER8" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="ER8" t="str">
+      <c r="ES8" t="str">
         <f>Tabelle1!AU8</f>
         <v>Beechcraft King Air 350i</v>
       </c>
     </row>
-    <row r="9" spans="1:148" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:149" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>88</v>
       </c>
@@ -11686,14 +11713,17 @@
         <v>88</v>
       </c>
       <c r="EQ9" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="ER9" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="ER9" t="str">
+      <c r="ES9" t="str">
         <f>Tabelle1!AU9</f>
         <v>Cessna 152</v>
       </c>
     </row>
-    <row r="10" spans="1:148" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:149" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
         <v>88</v>
       </c>
@@ -12170,14 +12200,17 @@
         <v>88</v>
       </c>
       <c r="EQ10" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="ER10" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="ER10" t="str">
+      <c r="ES10" t="str">
         <f>Tabelle1!AU10</f>
         <v>Cessna 152 Aero</v>
       </c>
     </row>
-    <row r="11" spans="1:148" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:149" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
         <v>88</v>
       </c>
@@ -12654,14 +12687,17 @@
         <v>88</v>
       </c>
       <c r="EQ11" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="ER11" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="ER11" t="str">
+      <c r="ES11" t="str">
         <f>Tabelle1!AU11</f>
         <v>Cessna 172sp Skyhawk G1000</v>
       </c>
     </row>
-    <row r="12" spans="1:148" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:149" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
         <v>88</v>
       </c>
@@ -13138,14 +13174,17 @@
         <v>88</v>
       </c>
       <c r="EQ12" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="ER12" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="ER12" t="str">
+      <c r="ES12" t="str">
         <f>Tabelle1!AU12</f>
         <v>Cessna 172sp Skyhawk</v>
       </c>
     </row>
-    <row r="13" spans="1:148" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:149" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
         <v>88</v>
       </c>
@@ -13622,14 +13661,17 @@
         <v>88</v>
       </c>
       <c r="EQ13" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="ER13" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="ER13" t="str">
+      <c r="ES13" t="str">
         <f>Tabelle1!AU13</f>
         <v>Cessna 208B Grand Caravan EX</v>
       </c>
     </row>
-    <row r="14" spans="1:148" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:149" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
         <v>88</v>
       </c>
@@ -14106,14 +14148,17 @@
         <v>88</v>
       </c>
       <c r="EQ14" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="ER14" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="ER14" t="str">
+      <c r="ES14" t="str">
         <f>Tabelle1!AU14</f>
         <v>Cessna CJ4 Citation</v>
       </c>
     </row>
-    <row r="15" spans="1:148" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:149" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
         <v>88</v>
       </c>
@@ -14590,14 +14635,17 @@
         <v>88</v>
       </c>
       <c r="EQ15" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="ER15" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="ER15" t="str">
+      <c r="ES15" t="str">
         <f>Tabelle1!AU15</f>
         <v>Cessna Longitude</v>
       </c>
     </row>
-    <row r="16" spans="1:148" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:149" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
         <v>88</v>
       </c>
@@ -15074,14 +15122,17 @@
         <v>88</v>
       </c>
       <c r="EQ16" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="ER16" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="ER16" t="str">
+      <c r="ES16" t="str">
         <f>Tabelle1!AU16</f>
         <v>DA40-NG</v>
       </c>
     </row>
-    <row r="17" spans="1:148" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:149" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
         <v>88</v>
       </c>
@@ -15558,14 +15609,17 @@
         <v>88</v>
       </c>
       <c r="EQ17" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="ER17" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="ER17" t="str">
+      <c r="ES17" t="str">
         <f>Tabelle1!AU17</f>
         <v>DA40 TDI</v>
       </c>
     </row>
-    <row r="18" spans="1:148" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:149" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
         <v>88</v>
       </c>
@@ -16042,14 +16096,17 @@
         <v>88</v>
       </c>
       <c r="EQ18" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="ER18" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="ER18" t="str">
+      <c r="ES18" t="str">
         <f>Tabelle1!AU18</f>
         <v>DA62</v>
       </c>
     </row>
-    <row r="19" spans="1:148" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:149" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
         <v>88</v>
       </c>
@@ -16526,14 +16583,17 @@
         <v>88</v>
       </c>
       <c r="EQ19" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="ER19" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="ER19" t="str">
+      <c r="ES19" t="str">
         <f>Tabelle1!AU19</f>
         <v>DR400</v>
       </c>
     </row>
-    <row r="20" spans="1:148" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:149" x14ac:dyDescent="0.25">
       <c r="A20" s="12" t="s">
         <v>88</v>
       </c>
@@ -17010,14 +17070,17 @@
         <v>88</v>
       </c>
       <c r="EQ20" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="ER20" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="ER20" t="str">
+      <c r="ES20" t="str">
         <f>Tabelle1!AU20</f>
         <v>DV20</v>
       </c>
     </row>
-    <row r="21" spans="1:148" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:149" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
         <v>88</v>
       </c>
@@ -17494,14 +17557,17 @@
         <v>88</v>
       </c>
       <c r="EQ21" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="ER21" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="ER21" t="str">
+      <c r="ES21" t="str">
         <f>Tabelle1!AU21</f>
         <v>Extra 330</v>
       </c>
     </row>
-    <row r="22" spans="1:148" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:149" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="s">
         <v>88</v>
       </c>
@@ -17978,14 +18044,17 @@
         <v>88</v>
       </c>
       <c r="EQ22" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="ER22" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="ER22" t="str">
+      <c r="ES22" t="str">
         <f>Tabelle1!AU22</f>
         <v>FlightDesignCT</v>
       </c>
     </row>
-    <row r="23" spans="1:148" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:149" x14ac:dyDescent="0.25">
       <c r="A23" s="12" t="s">
         <v>88</v>
       </c>
@@ -18462,14 +18531,17 @@
         <v>88</v>
       </c>
       <c r="EQ23" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="ER23" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="ER23" t="str">
+      <c r="ES23" t="str">
         <f>Tabelle1!AU23</f>
         <v>Icon A5</v>
       </c>
     </row>
-    <row r="24" spans="1:148" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:149" x14ac:dyDescent="0.25">
       <c r="A24" s="12" t="s">
         <v>88</v>
       </c>
@@ -18946,14 +19018,17 @@
         <v>88</v>
       </c>
       <c r="EQ24" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="ER24" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="ER24" t="str">
+      <c r="ES24" t="str">
         <f>Tabelle1!AU24</f>
         <v>Mudry Cap 10 C</v>
       </c>
     </row>
-    <row r="25" spans="1:148" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:149" x14ac:dyDescent="0.25">
       <c r="A25" s="12" t="s">
         <v>88</v>
       </c>
@@ -19430,14 +19505,17 @@
         <v>88</v>
       </c>
       <c r="EQ25" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="ER25" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="ER25" t="str">
+      <c r="ES25" t="str">
         <f>Tabelle1!AU25</f>
         <v>Pilatus PC-6 Gauge</v>
       </c>
     </row>
-    <row r="26" spans="1:148" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:149" x14ac:dyDescent="0.25">
       <c r="A26" s="12" t="s">
         <v>88</v>
       </c>
@@ -19914,14 +19992,17 @@
         <v>88</v>
       </c>
       <c r="EQ26" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="ER26" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="ER26" t="str">
+      <c r="ES26" t="str">
         <f>Tabelle1!AU26</f>
         <v>Pilatus PC-6 G950</v>
       </c>
     </row>
-    <row r="27" spans="1:148" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:149" x14ac:dyDescent="0.25">
       <c r="A27" s="12" t="s">
         <v>88</v>
       </c>
@@ -20398,14 +20479,17 @@
         <v>88</v>
       </c>
       <c r="EQ27" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="ER27" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="ER27" t="str">
+      <c r="ES27" t="str">
         <f>Tabelle1!AU27</f>
         <v>Pipistrel Alpha Electro</v>
       </c>
     </row>
-    <row r="28" spans="1:148" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:149" x14ac:dyDescent="0.25">
       <c r="A28" s="12" t="s">
         <v>88</v>
       </c>
@@ -20882,14 +20966,17 @@
         <v>88</v>
       </c>
       <c r="EQ28" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="ER28" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="ER28" t="str">
+      <c r="ES28" t="str">
         <f>Tabelle1!AU28</f>
         <v>Pitts Special 1S</v>
       </c>
     </row>
-    <row r="29" spans="1:148" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:149" x14ac:dyDescent="0.25">
       <c r="A29" s="12" t="s">
         <v>88</v>
       </c>
@@ -21366,14 +21453,17 @@
         <v>88</v>
       </c>
       <c r="EQ29" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="ER29" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="ER29" t="str">
+      <c r="ES29" t="str">
         <f>Tabelle1!AU29</f>
         <v>Pitts Special S2S</v>
       </c>
     </row>
-    <row r="30" spans="1:148" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:149" x14ac:dyDescent="0.25">
       <c r="A30" s="12" t="s">
         <v>88</v>
       </c>
@@ -21850,14 +21940,17 @@
         <v>88</v>
       </c>
       <c r="EQ30" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="ER30" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="ER30" t="str">
+      <c r="ES30" t="str">
         <f>Tabelle1!AU30</f>
         <v>Savage Cub</v>
       </c>
     </row>
-    <row r="31" spans="1:148" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:149" x14ac:dyDescent="0.25">
       <c r="A31" s="12" t="s">
         <v>88</v>
       </c>
@@ -22334,14 +22427,17 @@
         <v>88</v>
       </c>
       <c r="EQ31" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="ER31" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="ER31" t="str">
+      <c r="ES31" t="str">
         <f>Tabelle1!AU31</f>
         <v>Savage Shock Ultra</v>
       </c>
     </row>
-    <row r="32" spans="1:148" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:149" x14ac:dyDescent="0.25">
       <c r="A32" s="12" t="s">
         <v>88</v>
       </c>
@@ -22818,14 +22914,17 @@
         <v>88</v>
       </c>
       <c r="EQ32" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="ER32" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="ER32" t="str">
+      <c r="ES32" t="str">
         <f>Tabelle1!AU32</f>
         <v>SR22</v>
       </c>
     </row>
-    <row r="33" spans="1:148" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:149" x14ac:dyDescent="0.25">
       <c r="A33" s="12" t="s">
         <v>88</v>
       </c>
@@ -23302,14 +23401,17 @@
         <v>88</v>
       </c>
       <c r="EQ33" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="ER33" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="ER33" t="str">
+      <c r="ES33" t="str">
         <f>Tabelle1!AU33</f>
         <v>TBM 930</v>
       </c>
     </row>
-    <row r="34" spans="1:148" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:149" x14ac:dyDescent="0.25">
       <c r="A34" s="12" t="s">
         <v>88</v>
       </c>
@@ -23786,14 +23888,17 @@
         <v>88</v>
       </c>
       <c r="EQ34" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="ER34" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="ER34" t="str">
+      <c r="ES34" t="str">
         <f>Tabelle1!AU34</f>
         <v>Vertigo</v>
       </c>
     </row>
-    <row r="35" spans="1:148" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:149" x14ac:dyDescent="0.25">
       <c r="A35" s="12" t="s">
         <v>88</v>
       </c>
@@ -24270,14 +24375,17 @@
         <v>88</v>
       </c>
       <c r="EQ35" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="ER35" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="ER35" t="str">
+      <c r="ES35" t="str">
         <f>Tabelle1!AU35</f>
         <v>VL3</v>
       </c>
     </row>
-    <row r="36" spans="1:148" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:149" x14ac:dyDescent="0.25">
       <c r="A36" s="12" t="s">
         <v>88</v>
       </c>
@@ -24754,14 +24862,17 @@
         <v>88</v>
       </c>
       <c r="EQ36" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="ER36" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="ER36" t="str">
+      <c r="ES36" t="str">
         <f>Tabelle1!AU36</f>
         <v>Volocity</v>
       </c>
     </row>
-    <row r="37" spans="1:148" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:149" x14ac:dyDescent="0.25">
       <c r="A37" s="12" t="s">
         <v>88</v>
       </c>
@@ -25238,14 +25349,17 @@
         <v>88</v>
       </c>
       <c r="EQ37" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="ER37" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="ER37" t="str">
+      <c r="ES37" t="str">
         <f>Tabelle1!AU37</f>
         <v>NXCub</v>
       </c>
     </row>
-    <row r="38" spans="1:148" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:149" x14ac:dyDescent="0.25">
       <c r="A38" s="12" t="s">
         <v>88</v>
       </c>
@@ -25722,14 +25836,17 @@
         <v>88</v>
       </c>
       <c r="EQ38" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="ER38" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="ER38" t="str">
+      <c r="ES38" t="str">
         <f>Tabelle1!AU38</f>
         <v>XCub</v>
       </c>
     </row>
-    <row r="39" spans="1:148" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:149" x14ac:dyDescent="0.25">
       <c r="A39" s="12" t="s">
         <v>88</v>
       </c>
@@ -26206,14 +26323,17 @@
         <v>88</v>
       </c>
       <c r="EQ39" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="ER39" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="ER39" t="str">
+      <c r="ES39" t="str">
         <f>Tabelle1!AU39</f>
         <v>SWS Kodiak 100 II</v>
       </c>
     </row>
-    <row r="40" spans="1:148" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:149" x14ac:dyDescent="0.25">
       <c r="A40" s="12" t="s">
         <v>88</v>
       </c>
@@ -26690,9 +26810,12 @@
         <v>88</v>
       </c>
       <c r="EQ40" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="ER40" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="ER40" t="str">
+      <c r="ES40" t="str">
         <f>Tabelle1!AU40</f>
         <v>Generic Glider</v>
       </c>

</xml_diff>

<commit_message>
Build 70 intermediate push for testing - Add Support for some prettier Simbrief Flightplan types (LIDO, ACA, EZY, SWA, UAL2018) - Add Support to include Simbrief images in Flightplan PDF - Update Improverd Flightplan decoding from ext. formats - Update PDF/IMG Converter for Shelf replaced with WkHtmlToX library - Update Deploy Sound files in HudBar Temp folder (less stray files)
</commit_message>
<xml_diff>
--- a/FS20_HudBar/Config/EngineMerge.xlsx
+++ b/FS20_HudBar/Config/EngineMerge.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5209" uniqueCount="318">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5372" uniqueCount="322">
   <si>
     <t>ACFT</t>
   </si>
@@ -972,6 +972,18 @@
   </si>
   <si>
     <t>NAV2_OBS</t>
+  </si>
+  <si>
+    <t>USR_ALERT_1</t>
+  </si>
+  <si>
+    <t>USR_ALERT_2</t>
+  </si>
+  <si>
+    <t>USR_ALERT_3</t>
+  </si>
+  <si>
+    <t>THOOK</t>
   </si>
 </sst>
 </file>
@@ -7676,10 +7688,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:FD41"/>
+  <dimension ref="A1:FH41"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="CT1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="FF25" sqref="FF25"/>
+      <selection activeCell="FH9" sqref="FH9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7687,11 +7699,11 @@
     <col min="1" max="75" width="3.7109375" bestFit="1" customWidth="1"/>
     <col min="76" max="77" width="3.7109375" customWidth="1"/>
     <col min="78" max="86" width="3.7109375" bestFit="1" customWidth="1"/>
-    <col min="87" max="159" width="3.7109375" customWidth="1"/>
-    <col min="160" max="160" width="36.28515625" customWidth="1"/>
+    <col min="87" max="163" width="3.7109375" customWidth="1"/>
+    <col min="164" max="164" width="36.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:160" s="11" customFormat="1" ht="75.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:164" s="11" customFormat="1" ht="75.75" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>95</v>
       </c>
@@ -8167,13 +8179,25 @@
         <v>317</v>
       </c>
       <c r="FC1" s="11" t="s">
+        <v>318</v>
+      </c>
+      <c r="FD1" s="11" t="s">
+        <v>319</v>
+      </c>
+      <c r="FE1" s="11" t="s">
+        <v>320</v>
+      </c>
+      <c r="FF1" s="11" t="s">
+        <v>321</v>
+      </c>
+      <c r="FG1" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="FD1" t="s">
+      <c r="FH1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:160" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:164" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>88</v>
       </c>
@@ -8687,14 +8711,26 @@
         <v>88</v>
       </c>
       <c r="FC2" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FD2" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FE2" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FF2" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FG2" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="FD2" t="str">
+      <c r="FH2" t="str">
         <f>Tabelle1!AV2</f>
         <v>Airbus A320 Neo</v>
       </c>
     </row>
-    <row r="3" spans="1:160" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:164" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
         <v>88</v>
       </c>
@@ -9208,14 +9244,26 @@
         <v>88</v>
       </c>
       <c r="FC3" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FD3" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FE3" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FF3" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FG3" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="FD3" t="str">
+      <c r="FH3" t="str">
         <f>Tabelle1!AV3</f>
         <v>Boeing 747-8i</v>
       </c>
     </row>
-    <row r="4" spans="1:160" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:164" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
         <v>88</v>
       </c>
@@ -9729,14 +9777,26 @@
         <v>88</v>
       </c>
       <c r="FC4" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FD4" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FE4" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FF4" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FG4" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="FD4" t="str">
+      <c r="FH4" t="str">
         <f>Tabelle1!AV4</f>
         <v>Boeing 787-10</v>
       </c>
     </row>
-    <row r="5" spans="1:160" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:164" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>88</v>
       </c>
@@ -10250,14 +10310,26 @@
         <v>88</v>
       </c>
       <c r="FC5" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FD5" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FE5" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FF5" s="12">
+        <v>1</v>
+      </c>
+      <c r="FG5" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="FD5" t="str">
+      <c r="FH5" t="str">
         <f>Tabelle1!AV5</f>
         <v>Boeing F/A 18E Super Hornet</v>
       </c>
     </row>
-    <row r="6" spans="1:160" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:164" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>88</v>
       </c>
@@ -10771,14 +10843,26 @@
         <v>88</v>
       </c>
       <c r="FC6" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FD6" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FE6" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FF6" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FG6" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="FD6" t="str">
+      <c r="FH6" t="str">
         <f>Tabelle1!AV6</f>
         <v>Baron G58</v>
       </c>
     </row>
-    <row r="7" spans="1:160" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:164" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>88</v>
       </c>
@@ -11292,14 +11376,26 @@
         <v>88</v>
       </c>
       <c r="FC7" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FD7" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FE7" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FF7" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FG7" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="FD7" t="str">
+      <c r="FH7" t="str">
         <f>Tabelle1!AV7</f>
         <v>Bonanza G36</v>
       </c>
     </row>
-    <row r="8" spans="1:160" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:164" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>88</v>
       </c>
@@ -11813,14 +11909,26 @@
         <v>88</v>
       </c>
       <c r="FC8" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FD8" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FE8" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FF8" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FG8" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="FD8" t="str">
+      <c r="FH8" t="str">
         <f>Tabelle1!AV8</f>
         <v>Beechcraft King Air 350i</v>
       </c>
     </row>
-    <row r="9" spans="1:160" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:164" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>88</v>
       </c>
@@ -12334,14 +12442,26 @@
         <v>88</v>
       </c>
       <c r="FC9" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FD9" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FE9" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FF9" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FG9" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="FD9" t="str">
+      <c r="FH9" t="str">
         <f>Tabelle1!AV9</f>
         <v>Cessna 152</v>
       </c>
     </row>
-    <row r="10" spans="1:160" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:164" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
         <v>88</v>
       </c>
@@ -12855,14 +12975,26 @@
         <v>88</v>
       </c>
       <c r="FC10" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FD10" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FE10" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FF10" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FG10" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="FD10" t="str">
+      <c r="FH10" t="str">
         <f>Tabelle1!AV10</f>
         <v>Cessna 152 Aero</v>
       </c>
     </row>
-    <row r="11" spans="1:160" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:164" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
         <v>88</v>
       </c>
@@ -13376,14 +13508,26 @@
         <v>88</v>
       </c>
       <c r="FC11" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FD11" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FE11" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FF11" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FG11" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="FD11" t="str">
+      <c r="FH11" t="str">
         <f>Tabelle1!AV11</f>
         <v>Cessna 172sp Skyhawk G1000</v>
       </c>
     </row>
-    <row r="12" spans="1:160" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:164" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
         <v>88</v>
       </c>
@@ -13897,14 +14041,26 @@
         <v>88</v>
       </c>
       <c r="FC12" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FD12" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FE12" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FF12" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FG12" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="FD12" t="str">
+      <c r="FH12" t="str">
         <f>Tabelle1!AV12</f>
         <v>Cessna 172sp Skyhawk</v>
       </c>
     </row>
-    <row r="13" spans="1:160" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:164" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
         <v>88</v>
       </c>
@@ -14418,14 +14574,26 @@
         <v>88</v>
       </c>
       <c r="FC13" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FD13" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FE13" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FF13" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FG13" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="FD13" t="str">
+      <c r="FH13" t="str">
         <f>Tabelle1!AV13</f>
         <v>Cessna 208B Grand Caravan EX</v>
       </c>
     </row>
-    <row r="14" spans="1:160" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:164" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
         <v>88</v>
       </c>
@@ -14939,14 +15107,26 @@
         <v>88</v>
       </c>
       <c r="FC14" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FD14" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FE14" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FF14" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FG14" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="FD14" t="str">
+      <c r="FH14" t="str">
         <f>Tabelle1!AV14</f>
         <v>Cessna CJ4 Citation</v>
       </c>
     </row>
-    <row r="15" spans="1:160" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:164" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
         <v>88</v>
       </c>
@@ -15460,14 +15640,26 @@
         <v>88</v>
       </c>
       <c r="FC15" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FD15" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FE15" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FF15" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FG15" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="FD15" t="str">
+      <c r="FH15" t="str">
         <f>Tabelle1!AV15</f>
         <v>Cessna Longitude</v>
       </c>
     </row>
-    <row r="16" spans="1:160" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:164" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
         <v>88</v>
       </c>
@@ -15981,14 +16173,26 @@
         <v>88</v>
       </c>
       <c r="FC16" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FD16" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FE16" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FF16" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FG16" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="FD16" t="str">
+      <c r="FH16" t="str">
         <f>Tabelle1!AV16</f>
         <v>DA40-NG</v>
       </c>
     </row>
-    <row r="17" spans="1:160" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:164" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
         <v>88</v>
       </c>
@@ -16502,14 +16706,26 @@
         <v>88</v>
       </c>
       <c r="FC17" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FD17" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FE17" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FF17" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FG17" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="FD17" t="str">
+      <c r="FH17" t="str">
         <f>Tabelle1!AV17</f>
         <v>DA40 TDI</v>
       </c>
     </row>
-    <row r="18" spans="1:160" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:164" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
         <v>88</v>
       </c>
@@ -17023,14 +17239,26 @@
         <v>88</v>
       </c>
       <c r="FC18" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FD18" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FE18" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FF18" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FG18" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="FD18" t="str">
+      <c r="FH18" t="str">
         <f>Tabelle1!AV18</f>
         <v>DA62</v>
       </c>
     </row>
-    <row r="19" spans="1:160" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:164" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
         <v>88</v>
       </c>
@@ -17544,14 +17772,26 @@
         <v>88</v>
       </c>
       <c r="FC19" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FD19" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FE19" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FF19" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FG19" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="FD19" t="str">
+      <c r="FH19" t="str">
         <f>Tabelle1!AV19</f>
         <v>DR400</v>
       </c>
     </row>
-    <row r="20" spans="1:160" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:164" x14ac:dyDescent="0.25">
       <c r="A20" s="12" t="s">
         <v>88</v>
       </c>
@@ -18065,14 +18305,26 @@
         <v>88</v>
       </c>
       <c r="FC20" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FD20" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FE20" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FF20" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FG20" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="FD20" t="str">
+      <c r="FH20" t="str">
         <f>Tabelle1!AV20</f>
         <v>DV20</v>
       </c>
     </row>
-    <row r="21" spans="1:160" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:164" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
         <v>88</v>
       </c>
@@ -18586,14 +18838,26 @@
         <v>88</v>
       </c>
       <c r="FC21" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FD21" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FE21" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FF21" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FG21" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="FD21" t="str">
+      <c r="FH21" t="str">
         <f>Tabelle1!AV21</f>
         <v>Extra 330</v>
       </c>
     </row>
-    <row r="22" spans="1:160" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:164" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="s">
         <v>88</v>
       </c>
@@ -19107,14 +19371,26 @@
         <v>88</v>
       </c>
       <c r="FC22" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FD22" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FE22" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FF22" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FG22" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="FD22" t="str">
+      <c r="FH22" t="str">
         <f>Tabelle1!AV22</f>
         <v>FlightDesignCT</v>
       </c>
     </row>
-    <row r="23" spans="1:160" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:164" x14ac:dyDescent="0.25">
       <c r="A23" s="12" t="s">
         <v>88</v>
       </c>
@@ -19628,14 +19904,26 @@
         <v>88</v>
       </c>
       <c r="FC23" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FD23" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FE23" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FF23" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FG23" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="FD23" t="str">
+      <c r="FH23" t="str">
         <f>Tabelle1!AV23</f>
         <v>Icon A5</v>
       </c>
     </row>
-    <row r="24" spans="1:160" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:164" x14ac:dyDescent="0.25">
       <c r="A24" s="12" t="s">
         <v>88</v>
       </c>
@@ -20149,14 +20437,26 @@
         <v>88</v>
       </c>
       <c r="FC24" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FD24" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FE24" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FF24" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FG24" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="FD24" t="str">
+      <c r="FH24" t="str">
         <f>Tabelle1!AV24</f>
         <v>Mudry Cap 10 C</v>
       </c>
     </row>
-    <row r="25" spans="1:160" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:164" x14ac:dyDescent="0.25">
       <c r="A25" s="12" t="s">
         <v>88</v>
       </c>
@@ -20670,14 +20970,26 @@
         <v>88</v>
       </c>
       <c r="FC25" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FD25" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FE25" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FF25" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FG25" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="FD25" t="str">
+      <c r="FH25" t="str">
         <f>Tabelle1!AV25</f>
         <v>Pilatus PC-6 Gauge</v>
       </c>
     </row>
-    <row r="26" spans="1:160" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:164" x14ac:dyDescent="0.25">
       <c r="A26" s="12" t="s">
         <v>88</v>
       </c>
@@ -21191,14 +21503,26 @@
         <v>88</v>
       </c>
       <c r="FC26" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FD26" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FE26" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FF26" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FG26" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="FD26" t="str">
+      <c r="FH26" t="str">
         <f>Tabelle1!AV26</f>
         <v>Pilatus PC-6 G950</v>
       </c>
     </row>
-    <row r="27" spans="1:160" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:164" x14ac:dyDescent="0.25">
       <c r="A27" s="12" t="s">
         <v>88</v>
       </c>
@@ -21712,14 +22036,26 @@
         <v>88</v>
       </c>
       <c r="FC27" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FD27" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FE27" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FF27" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FG27" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="FD27" t="str">
+      <c r="FH27" t="str">
         <f>Tabelle1!AV27</f>
         <v>Pipistrel Alpha Electro</v>
       </c>
     </row>
-    <row r="28" spans="1:160" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:164" x14ac:dyDescent="0.25">
       <c r="A28" s="12" t="s">
         <v>88</v>
       </c>
@@ -22233,14 +22569,26 @@
         <v>88</v>
       </c>
       <c r="FC28" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FD28" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FE28" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FF28" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FG28" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="FD28" t="str">
+      <c r="FH28" t="str">
         <f>Tabelle1!AV28</f>
         <v>Pitts Special 1S</v>
       </c>
     </row>
-    <row r="29" spans="1:160" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:164" x14ac:dyDescent="0.25">
       <c r="A29" s="12" t="s">
         <v>88</v>
       </c>
@@ -22754,14 +23102,26 @@
         <v>88</v>
       </c>
       <c r="FC29" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FD29" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FE29" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FF29" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FG29" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="FD29" t="str">
+      <c r="FH29" t="str">
         <f>Tabelle1!AV29</f>
         <v>Pitts Special S2S</v>
       </c>
     </row>
-    <row r="30" spans="1:160" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:164" x14ac:dyDescent="0.25">
       <c r="A30" s="12" t="s">
         <v>88</v>
       </c>
@@ -23275,14 +23635,26 @@
         <v>88</v>
       </c>
       <c r="FC30" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FD30" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FE30" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FF30" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FG30" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="FD30" t="str">
+      <c r="FH30" t="str">
         <f>Tabelle1!AV30</f>
         <v>Savage Cub</v>
       </c>
     </row>
-    <row r="31" spans="1:160" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:164" x14ac:dyDescent="0.25">
       <c r="A31" s="12" t="s">
         <v>88</v>
       </c>
@@ -23796,14 +24168,26 @@
         <v>88</v>
       </c>
       <c r="FC31" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FD31" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FE31" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FF31" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FG31" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="FD31" t="str">
+      <c r="FH31" t="str">
         <f>Tabelle1!AV31</f>
         <v>Savage Shock Ultra</v>
       </c>
     </row>
-    <row r="32" spans="1:160" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:164" x14ac:dyDescent="0.25">
       <c r="A32" s="12" t="s">
         <v>88</v>
       </c>
@@ -24317,14 +24701,26 @@
         <v>88</v>
       </c>
       <c r="FC32" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FD32" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FE32" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FF32" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FG32" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="FD32" t="str">
+      <c r="FH32" t="str">
         <f>Tabelle1!AV32</f>
         <v>SR22</v>
       </c>
     </row>
-    <row r="33" spans="1:160" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:164" x14ac:dyDescent="0.25">
       <c r="A33" s="12" t="s">
         <v>88</v>
       </c>
@@ -24838,14 +25234,26 @@
         <v>88</v>
       </c>
       <c r="FC33" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FD33" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FE33" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FF33" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FG33" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="FD33" t="str">
+      <c r="FH33" t="str">
         <f>Tabelle1!AV33</f>
         <v>TBM 930</v>
       </c>
     </row>
-    <row r="34" spans="1:160" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:164" x14ac:dyDescent="0.25">
       <c r="A34" s="12" t="s">
         <v>88</v>
       </c>
@@ -25359,14 +25767,26 @@
         <v>88</v>
       </c>
       <c r="FC34" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FD34" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FE34" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FF34" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FG34" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="FD34" t="str">
+      <c r="FH34" t="str">
         <f>Tabelle1!AV34</f>
         <v>Vertigo</v>
       </c>
     </row>
-    <row r="35" spans="1:160" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:164" x14ac:dyDescent="0.25">
       <c r="A35" s="12" t="s">
         <v>88</v>
       </c>
@@ -25880,14 +26300,26 @@
         <v>88</v>
       </c>
       <c r="FC35" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FD35" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FE35" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FF35" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FG35" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="FD35" t="str">
+      <c r="FH35" t="str">
         <f>Tabelle1!AV35</f>
         <v>VL3</v>
       </c>
     </row>
-    <row r="36" spans="1:160" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:164" x14ac:dyDescent="0.25">
       <c r="A36" s="12" t="s">
         <v>88</v>
       </c>
@@ -26401,14 +26833,26 @@
         <v>88</v>
       </c>
       <c r="FC36" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FD36" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FE36" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FF36" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FG36" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="FD36" t="str">
+      <c r="FH36" t="str">
         <f>Tabelle1!AV36</f>
         <v>Volocity</v>
       </c>
     </row>
-    <row r="37" spans="1:160" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:164" x14ac:dyDescent="0.25">
       <c r="A37" s="12" t="s">
         <v>88</v>
       </c>
@@ -26922,14 +27366,26 @@
         <v>88</v>
       </c>
       <c r="FC37" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FD37" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FE37" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FF37" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FG37" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="FD37" t="str">
+      <c r="FH37" t="str">
         <f>Tabelle1!AV37</f>
         <v>NXCub</v>
       </c>
     </row>
-    <row r="38" spans="1:160" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:164" x14ac:dyDescent="0.25">
       <c r="A38" s="12" t="s">
         <v>88</v>
       </c>
@@ -27443,14 +27899,26 @@
         <v>88</v>
       </c>
       <c r="FC38" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FD38" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FE38" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FF38" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FG38" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="FD38" t="str">
+      <c r="FH38" t="str">
         <f>Tabelle1!AV38</f>
         <v>XCub</v>
       </c>
     </row>
-    <row r="39" spans="1:160" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:164" x14ac:dyDescent="0.25">
       <c r="A39" s="12" t="s">
         <v>88</v>
       </c>
@@ -27964,14 +28432,26 @@
         <v>88</v>
       </c>
       <c r="FC39" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FD39" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FE39" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FF39" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FG39" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="FD39" t="str">
+      <c r="FH39" t="str">
         <f>Tabelle1!AV39</f>
         <v>SWS Kodiak 100 II</v>
       </c>
     </row>
-    <row r="40" spans="1:160" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:164" x14ac:dyDescent="0.25">
       <c r="A40" s="12" t="s">
         <v>88</v>
       </c>
@@ -28485,14 +28965,26 @@
         <v>88</v>
       </c>
       <c r="FC40" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FD40" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FE40" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FF40" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FG40" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="FD40" t="str">
+      <c r="FH40" t="str">
         <f>Tabelle1!AV40</f>
         <v>Generic Glider</v>
       </c>
     </row>
-    <row r="41" spans="1:160" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:164" x14ac:dyDescent="0.25">
       <c r="A41" s="12" t="s">
         <v>88</v>
       </c>
@@ -29006,9 +29498,21 @@
         <v>88</v>
       </c>
       <c r="FC41" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FD41" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FE41" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FF41" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FG41" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="FD41" t="str">
+      <c r="FH41" t="str">
         <f>Tabelle1!AV41</f>
         <v>Generic Heli Turbine</v>
       </c>

</xml_diff>

<commit_message>
Add Collective Handle Position V0.72 testing now
</commit_message>
<xml_diff>
--- a/FS20_HudBar/Config/EngineMerge.xlsx
+++ b/FS20_HudBar/Config/EngineMerge.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5372" uniqueCount="322">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5374" uniqueCount="324">
   <si>
     <t>ACFT</t>
   </si>
@@ -984,6 +984,12 @@
   </si>
   <si>
     <t>THOOK</t>
+  </si>
+  <si>
+    <t>SBALL_ANI</t>
+  </si>
+  <si>
+    <t>H_COLL_LEV</t>
   </si>
 </sst>
 </file>
@@ -7688,10 +7694,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:FH41"/>
+  <dimension ref="A1:FJ41"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="CT1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="FH9" sqref="FH9"/>
+      <selection activeCell="EU26" sqref="EU26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7699,11 +7705,11 @@
     <col min="1" max="75" width="3.7109375" bestFit="1" customWidth="1"/>
     <col min="76" max="77" width="3.7109375" customWidth="1"/>
     <col min="78" max="86" width="3.7109375" bestFit="1" customWidth="1"/>
-    <col min="87" max="163" width="3.7109375" customWidth="1"/>
-    <col min="164" max="164" width="36.28515625" customWidth="1"/>
+    <col min="87" max="165" width="3.7109375" customWidth="1"/>
+    <col min="166" max="166" width="36.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:164" s="11" customFormat="1" ht="75.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:166" s="11" customFormat="1" ht="75.75" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>95</v>
       </c>
@@ -8191,13 +8197,19 @@
         <v>321</v>
       </c>
       <c r="FG1" s="11" t="s">
+        <v>322</v>
+      </c>
+      <c r="FH1" s="11" t="s">
+        <v>323</v>
+      </c>
+      <c r="FI1" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="FH1" t="s">
+      <c r="FJ1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:164" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:166" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>88</v>
       </c>
@@ -8686,8 +8698,8 @@
       <c r="ET2" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="EU2" s="12" t="s">
-        <v>88</v>
+      <c r="EU2" s="12">
+        <v>0</v>
       </c>
       <c r="EV2" s="12" t="s">
         <v>88</v>
@@ -8723,14 +8735,20 @@
         <v>88</v>
       </c>
       <c r="FG2" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FH2" s="12">
+        <v>0</v>
+      </c>
+      <c r="FI2" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="FH2" t="str">
+      <c r="FJ2" t="str">
         <f>Tabelle1!AV2</f>
         <v>Airbus A320 Neo</v>
       </c>
     </row>
-    <row r="3" spans="1:164" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:166" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
         <v>88</v>
       </c>
@@ -9219,8 +9237,8 @@
       <c r="ET3" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="EU3" s="12" t="s">
-        <v>88</v>
+      <c r="EU3" s="12">
+        <v>0</v>
       </c>
       <c r="EV3" s="12" t="s">
         <v>88</v>
@@ -9256,14 +9274,20 @@
         <v>88</v>
       </c>
       <c r="FG3" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FH3" s="12">
+        <v>0</v>
+      </c>
+      <c r="FI3" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="FH3" t="str">
+      <c r="FJ3" t="str">
         <f>Tabelle1!AV3</f>
         <v>Boeing 747-8i</v>
       </c>
     </row>
-    <row r="4" spans="1:164" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:166" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
         <v>88</v>
       </c>
@@ -9752,8 +9776,8 @@
       <c r="ET4" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="EU4" s="12" t="s">
-        <v>88</v>
+      <c r="EU4" s="12">
+        <v>0</v>
       </c>
       <c r="EV4" s="12" t="s">
         <v>88</v>
@@ -9789,14 +9813,20 @@
         <v>88</v>
       </c>
       <c r="FG4" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FH4" s="12">
+        <v>0</v>
+      </c>
+      <c r="FI4" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="FH4" t="str">
+      <c r="FJ4" t="str">
         <f>Tabelle1!AV4</f>
         <v>Boeing 787-10</v>
       </c>
     </row>
-    <row r="5" spans="1:164" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:166" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>88</v>
       </c>
@@ -10285,8 +10315,8 @@
       <c r="ET5" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="EU5" s="12" t="s">
-        <v>88</v>
+      <c r="EU5" s="12">
+        <v>0</v>
       </c>
       <c r="EV5" s="12" t="s">
         <v>88</v>
@@ -10322,14 +10352,20 @@
         <v>1</v>
       </c>
       <c r="FG5" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FH5" s="12">
+        <v>0</v>
+      </c>
+      <c r="FI5" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="FH5" t="str">
+      <c r="FJ5" t="str">
         <f>Tabelle1!AV5</f>
         <v>Boeing F/A 18E Super Hornet</v>
       </c>
     </row>
-    <row r="6" spans="1:164" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:166" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>88</v>
       </c>
@@ -10818,8 +10854,8 @@
       <c r="ET6" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="EU6" s="12" t="s">
-        <v>88</v>
+      <c r="EU6" s="12">
+        <v>0</v>
       </c>
       <c r="EV6" s="12" t="s">
         <v>88</v>
@@ -10855,14 +10891,20 @@
         <v>88</v>
       </c>
       <c r="FG6" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FH6" s="12">
+        <v>0</v>
+      </c>
+      <c r="FI6" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="FH6" t="str">
+      <c r="FJ6" t="str">
         <f>Tabelle1!AV6</f>
         <v>Baron G58</v>
       </c>
     </row>
-    <row r="7" spans="1:164" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:166" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>88</v>
       </c>
@@ -11351,8 +11393,8 @@
       <c r="ET7" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="EU7" s="12" t="s">
-        <v>88</v>
+      <c r="EU7" s="12">
+        <v>0</v>
       </c>
       <c r="EV7" s="12" t="s">
         <v>88</v>
@@ -11388,14 +11430,20 @@
         <v>88</v>
       </c>
       <c r="FG7" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FH7" s="12">
+        <v>0</v>
+      </c>
+      <c r="FI7" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="FH7" t="str">
+      <c r="FJ7" t="str">
         <f>Tabelle1!AV7</f>
         <v>Bonanza G36</v>
       </c>
     </row>
-    <row r="8" spans="1:164" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:166" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>88</v>
       </c>
@@ -11884,8 +11932,8 @@
       <c r="ET8" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="EU8" s="12" t="s">
-        <v>88</v>
+      <c r="EU8" s="12">
+        <v>0</v>
       </c>
       <c r="EV8" s="12" t="s">
         <v>88</v>
@@ -11921,14 +11969,20 @@
         <v>88</v>
       </c>
       <c r="FG8" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FH8" s="12">
+        <v>0</v>
+      </c>
+      <c r="FI8" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="FH8" t="str">
+      <c r="FJ8" t="str">
         <f>Tabelle1!AV8</f>
         <v>Beechcraft King Air 350i</v>
       </c>
     </row>
-    <row r="9" spans="1:164" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:166" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>88</v>
       </c>
@@ -12417,8 +12471,8 @@
       <c r="ET9" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="EU9" s="12" t="s">
-        <v>88</v>
+      <c r="EU9" s="12">
+        <v>0</v>
       </c>
       <c r="EV9" s="12" t="s">
         <v>88</v>
@@ -12454,14 +12508,20 @@
         <v>88</v>
       </c>
       <c r="FG9" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FH9" s="12">
+        <v>0</v>
+      </c>
+      <c r="FI9" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="FH9" t="str">
+      <c r="FJ9" t="str">
         <f>Tabelle1!AV9</f>
         <v>Cessna 152</v>
       </c>
     </row>
-    <row r="10" spans="1:164" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:166" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
         <v>88</v>
       </c>
@@ -12950,8 +13010,8 @@
       <c r="ET10" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="EU10" s="12" t="s">
-        <v>88</v>
+      <c r="EU10" s="12">
+        <v>0</v>
       </c>
       <c r="EV10" s="12" t="s">
         <v>88</v>
@@ -12987,14 +13047,20 @@
         <v>88</v>
       </c>
       <c r="FG10" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FH10" s="12">
+        <v>0</v>
+      </c>
+      <c r="FI10" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="FH10" t="str">
+      <c r="FJ10" t="str">
         <f>Tabelle1!AV10</f>
         <v>Cessna 152 Aero</v>
       </c>
     </row>
-    <row r="11" spans="1:164" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:166" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
         <v>88</v>
       </c>
@@ -13483,8 +13549,8 @@
       <c r="ET11" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="EU11" s="12" t="s">
-        <v>88</v>
+      <c r="EU11" s="12">
+        <v>0</v>
       </c>
       <c r="EV11" s="12" t="s">
         <v>88</v>
@@ -13520,14 +13586,20 @@
         <v>88</v>
       </c>
       <c r="FG11" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FH11" s="12">
+        <v>0</v>
+      </c>
+      <c r="FI11" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="FH11" t="str">
+      <c r="FJ11" t="str">
         <f>Tabelle1!AV11</f>
         <v>Cessna 172sp Skyhawk G1000</v>
       </c>
     </row>
-    <row r="12" spans="1:164" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:166" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
         <v>88</v>
       </c>
@@ -14016,8 +14088,8 @@
       <c r="ET12" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="EU12" s="12" t="s">
-        <v>88</v>
+      <c r="EU12" s="12">
+        <v>0</v>
       </c>
       <c r="EV12" s="12" t="s">
         <v>88</v>
@@ -14053,14 +14125,20 @@
         <v>88</v>
       </c>
       <c r="FG12" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FH12" s="12">
+        <v>0</v>
+      </c>
+      <c r="FI12" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="FH12" t="str">
+      <c r="FJ12" t="str">
         <f>Tabelle1!AV12</f>
         <v>Cessna 172sp Skyhawk</v>
       </c>
     </row>
-    <row r="13" spans="1:164" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:166" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
         <v>88</v>
       </c>
@@ -14549,8 +14627,8 @@
       <c r="ET13" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="EU13" s="12" t="s">
-        <v>88</v>
+      <c r="EU13" s="12">
+        <v>0</v>
       </c>
       <c r="EV13" s="12" t="s">
         <v>88</v>
@@ -14586,14 +14664,20 @@
         <v>88</v>
       </c>
       <c r="FG13" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FH13" s="12">
+        <v>0</v>
+      </c>
+      <c r="FI13" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="FH13" t="str">
+      <c r="FJ13" t="str">
         <f>Tabelle1!AV13</f>
         <v>Cessna 208B Grand Caravan EX</v>
       </c>
     </row>
-    <row r="14" spans="1:164" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:166" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
         <v>88</v>
       </c>
@@ -15082,8 +15166,8 @@
       <c r="ET14" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="EU14" s="12" t="s">
-        <v>88</v>
+      <c r="EU14" s="12">
+        <v>0</v>
       </c>
       <c r="EV14" s="12" t="s">
         <v>88</v>
@@ -15119,14 +15203,20 @@
         <v>88</v>
       </c>
       <c r="FG14" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FH14" s="12">
+        <v>0</v>
+      </c>
+      <c r="FI14" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="FH14" t="str">
+      <c r="FJ14" t="str">
         <f>Tabelle1!AV14</f>
         <v>Cessna CJ4 Citation</v>
       </c>
     </row>
-    <row r="15" spans="1:164" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:166" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
         <v>88</v>
       </c>
@@ -15615,8 +15705,8 @@
       <c r="ET15" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="EU15" s="12" t="s">
-        <v>88</v>
+      <c r="EU15" s="12">
+        <v>0</v>
       </c>
       <c r="EV15" s="12" t="s">
         <v>88</v>
@@ -15652,14 +15742,20 @@
         <v>88</v>
       </c>
       <c r="FG15" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FH15" s="12">
+        <v>0</v>
+      </c>
+      <c r="FI15" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="FH15" t="str">
+      <c r="FJ15" t="str">
         <f>Tabelle1!AV15</f>
         <v>Cessna Longitude</v>
       </c>
     </row>
-    <row r="16" spans="1:164" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:166" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
         <v>88</v>
       </c>
@@ -16148,8 +16244,8 @@
       <c r="ET16" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="EU16" s="12" t="s">
-        <v>88</v>
+      <c r="EU16" s="12">
+        <v>0</v>
       </c>
       <c r="EV16" s="12" t="s">
         <v>88</v>
@@ -16185,14 +16281,20 @@
         <v>88</v>
       </c>
       <c r="FG16" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FH16" s="12">
+        <v>0</v>
+      </c>
+      <c r="FI16" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="FH16" t="str">
+      <c r="FJ16" t="str">
         <f>Tabelle1!AV16</f>
         <v>DA40-NG</v>
       </c>
     </row>
-    <row r="17" spans="1:164" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:166" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
         <v>88</v>
       </c>
@@ -16681,8 +16783,8 @@
       <c r="ET17" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="EU17" s="12" t="s">
-        <v>88</v>
+      <c r="EU17" s="12">
+        <v>0</v>
       </c>
       <c r="EV17" s="12" t="s">
         <v>88</v>
@@ -16718,14 +16820,20 @@
         <v>88</v>
       </c>
       <c r="FG17" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FH17" s="12">
+        <v>0</v>
+      </c>
+      <c r="FI17" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="FH17" t="str">
+      <c r="FJ17" t="str">
         <f>Tabelle1!AV17</f>
         <v>DA40 TDI</v>
       </c>
     </row>
-    <row r="18" spans="1:164" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:166" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
         <v>88</v>
       </c>
@@ -17214,8 +17322,8 @@
       <c r="ET18" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="EU18" s="12" t="s">
-        <v>88</v>
+      <c r="EU18" s="12">
+        <v>0</v>
       </c>
       <c r="EV18" s="12" t="s">
         <v>88</v>
@@ -17251,14 +17359,20 @@
         <v>88</v>
       </c>
       <c r="FG18" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FH18" s="12">
+        <v>0</v>
+      </c>
+      <c r="FI18" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="FH18" t="str">
+      <c r="FJ18" t="str">
         <f>Tabelle1!AV18</f>
         <v>DA62</v>
       </c>
     </row>
-    <row r="19" spans="1:164" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:166" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
         <v>88</v>
       </c>
@@ -17747,8 +17861,8 @@
       <c r="ET19" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="EU19" s="12" t="s">
-        <v>88</v>
+      <c r="EU19" s="12">
+        <v>0</v>
       </c>
       <c r="EV19" s="12" t="s">
         <v>88</v>
@@ -17784,14 +17898,20 @@
         <v>88</v>
       </c>
       <c r="FG19" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FH19" s="12">
+        <v>0</v>
+      </c>
+      <c r="FI19" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="FH19" t="str">
+      <c r="FJ19" t="str">
         <f>Tabelle1!AV19</f>
         <v>DR400</v>
       </c>
     </row>
-    <row r="20" spans="1:164" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:166" x14ac:dyDescent="0.25">
       <c r="A20" s="12" t="s">
         <v>88</v>
       </c>
@@ -18280,8 +18400,8 @@
       <c r="ET20" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="EU20" s="12" t="s">
-        <v>88</v>
+      <c r="EU20" s="12">
+        <v>0</v>
       </c>
       <c r="EV20" s="12" t="s">
         <v>88</v>
@@ -18317,14 +18437,20 @@
         <v>88</v>
       </c>
       <c r="FG20" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FH20" s="12">
+        <v>0</v>
+      </c>
+      <c r="FI20" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="FH20" t="str">
+      <c r="FJ20" t="str">
         <f>Tabelle1!AV20</f>
         <v>DV20</v>
       </c>
     </row>
-    <row r="21" spans="1:164" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:166" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
         <v>88</v>
       </c>
@@ -18813,8 +18939,8 @@
       <c r="ET21" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="EU21" s="12" t="s">
-        <v>88</v>
+      <c r="EU21" s="12">
+        <v>0</v>
       </c>
       <c r="EV21" s="12" t="s">
         <v>88</v>
@@ -18850,14 +18976,20 @@
         <v>88</v>
       </c>
       <c r="FG21" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FH21" s="12">
+        <v>0</v>
+      </c>
+      <c r="FI21" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="FH21" t="str">
+      <c r="FJ21" t="str">
         <f>Tabelle1!AV21</f>
         <v>Extra 330</v>
       </c>
     </row>
-    <row r="22" spans="1:164" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:166" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="s">
         <v>88</v>
       </c>
@@ -19346,8 +19478,8 @@
       <c r="ET22" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="EU22" s="12" t="s">
-        <v>88</v>
+      <c r="EU22" s="12">
+        <v>0</v>
       </c>
       <c r="EV22" s="12" t="s">
         <v>88</v>
@@ -19383,14 +19515,20 @@
         <v>88</v>
       </c>
       <c r="FG22" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FH22" s="12">
+        <v>0</v>
+      </c>
+      <c r="FI22" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="FH22" t="str">
+      <c r="FJ22" t="str">
         <f>Tabelle1!AV22</f>
         <v>FlightDesignCT</v>
       </c>
     </row>
-    <row r="23" spans="1:164" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:166" x14ac:dyDescent="0.25">
       <c r="A23" s="12" t="s">
         <v>88</v>
       </c>
@@ -19879,8 +20017,8 @@
       <c r="ET23" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="EU23" s="12" t="s">
-        <v>88</v>
+      <c r="EU23" s="12">
+        <v>0</v>
       </c>
       <c r="EV23" s="12" t="s">
         <v>88</v>
@@ -19916,14 +20054,20 @@
         <v>88</v>
       </c>
       <c r="FG23" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FH23" s="12">
+        <v>0</v>
+      </c>
+      <c r="FI23" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="FH23" t="str">
+      <c r="FJ23" t="str">
         <f>Tabelle1!AV23</f>
         <v>Icon A5</v>
       </c>
     </row>
-    <row r="24" spans="1:164" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:166" x14ac:dyDescent="0.25">
       <c r="A24" s="12" t="s">
         <v>88</v>
       </c>
@@ -20412,8 +20556,8 @@
       <c r="ET24" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="EU24" s="12" t="s">
-        <v>88</v>
+      <c r="EU24" s="12">
+        <v>0</v>
       </c>
       <c r="EV24" s="12" t="s">
         <v>88</v>
@@ -20449,14 +20593,20 @@
         <v>88</v>
       </c>
       <c r="FG24" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FH24" s="12">
+        <v>0</v>
+      </c>
+      <c r="FI24" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="FH24" t="str">
+      <c r="FJ24" t="str">
         <f>Tabelle1!AV24</f>
         <v>Mudry Cap 10 C</v>
       </c>
     </row>
-    <row r="25" spans="1:164" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:166" x14ac:dyDescent="0.25">
       <c r="A25" s="12" t="s">
         <v>88</v>
       </c>
@@ -20945,8 +21095,8 @@
       <c r="ET25" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="EU25" s="12" t="s">
-        <v>88</v>
+      <c r="EU25" s="12">
+        <v>0</v>
       </c>
       <c r="EV25" s="12" t="s">
         <v>88</v>
@@ -20982,14 +21132,20 @@
         <v>88</v>
       </c>
       <c r="FG25" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FH25" s="12">
+        <v>0</v>
+      </c>
+      <c r="FI25" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="FH25" t="str">
+      <c r="FJ25" t="str">
         <f>Tabelle1!AV25</f>
         <v>Pilatus PC-6 Gauge</v>
       </c>
     </row>
-    <row r="26" spans="1:164" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:166" x14ac:dyDescent="0.25">
       <c r="A26" s="12" t="s">
         <v>88</v>
       </c>
@@ -21478,8 +21634,8 @@
       <c r="ET26" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="EU26" s="12" t="s">
-        <v>88</v>
+      <c r="EU26" s="12">
+        <v>0</v>
       </c>
       <c r="EV26" s="12" t="s">
         <v>88</v>
@@ -21515,14 +21671,20 @@
         <v>88</v>
       </c>
       <c r="FG26" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FH26" s="12">
+        <v>0</v>
+      </c>
+      <c r="FI26" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="FH26" t="str">
+      <c r="FJ26" t="str">
         <f>Tabelle1!AV26</f>
         <v>Pilatus PC-6 G950</v>
       </c>
     </row>
-    <row r="27" spans="1:164" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:166" x14ac:dyDescent="0.25">
       <c r="A27" s="12" t="s">
         <v>88</v>
       </c>
@@ -22011,8 +22173,8 @@
       <c r="ET27" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="EU27" s="12" t="s">
-        <v>88</v>
+      <c r="EU27" s="12">
+        <v>0</v>
       </c>
       <c r="EV27" s="12" t="s">
         <v>88</v>
@@ -22048,14 +22210,20 @@
         <v>88</v>
       </c>
       <c r="FG27" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FH27" s="12">
+        <v>0</v>
+      </c>
+      <c r="FI27" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="FH27" t="str">
+      <c r="FJ27" t="str">
         <f>Tabelle1!AV27</f>
         <v>Pipistrel Alpha Electro</v>
       </c>
     </row>
-    <row r="28" spans="1:164" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:166" x14ac:dyDescent="0.25">
       <c r="A28" s="12" t="s">
         <v>88</v>
       </c>
@@ -22544,8 +22712,8 @@
       <c r="ET28" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="EU28" s="12" t="s">
-        <v>88</v>
+      <c r="EU28" s="12">
+        <v>0</v>
       </c>
       <c r="EV28" s="12" t="s">
         <v>88</v>
@@ -22581,14 +22749,20 @@
         <v>88</v>
       </c>
       <c r="FG28" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FH28" s="12">
+        <v>0</v>
+      </c>
+      <c r="FI28" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="FH28" t="str">
+      <c r="FJ28" t="str">
         <f>Tabelle1!AV28</f>
         <v>Pitts Special 1S</v>
       </c>
     </row>
-    <row r="29" spans="1:164" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:166" x14ac:dyDescent="0.25">
       <c r="A29" s="12" t="s">
         <v>88</v>
       </c>
@@ -23077,8 +23251,8 @@
       <c r="ET29" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="EU29" s="12" t="s">
-        <v>88</v>
+      <c r="EU29" s="12">
+        <v>0</v>
       </c>
       <c r="EV29" s="12" t="s">
         <v>88</v>
@@ -23114,14 +23288,20 @@
         <v>88</v>
       </c>
       <c r="FG29" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FH29" s="12">
+        <v>0</v>
+      </c>
+      <c r="FI29" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="FH29" t="str">
+      <c r="FJ29" t="str">
         <f>Tabelle1!AV29</f>
         <v>Pitts Special S2S</v>
       </c>
     </row>
-    <row r="30" spans="1:164" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:166" x14ac:dyDescent="0.25">
       <c r="A30" s="12" t="s">
         <v>88</v>
       </c>
@@ -23610,8 +23790,8 @@
       <c r="ET30" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="EU30" s="12" t="s">
-        <v>88</v>
+      <c r="EU30" s="12">
+        <v>0</v>
       </c>
       <c r="EV30" s="12" t="s">
         <v>88</v>
@@ -23647,14 +23827,20 @@
         <v>88</v>
       </c>
       <c r="FG30" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FH30" s="12">
+        <v>0</v>
+      </c>
+      <c r="FI30" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="FH30" t="str">
+      <c r="FJ30" t="str">
         <f>Tabelle1!AV30</f>
         <v>Savage Cub</v>
       </c>
     </row>
-    <row r="31" spans="1:164" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:166" x14ac:dyDescent="0.25">
       <c r="A31" s="12" t="s">
         <v>88</v>
       </c>
@@ -24143,8 +24329,8 @@
       <c r="ET31" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="EU31" s="12" t="s">
-        <v>88</v>
+      <c r="EU31" s="12">
+        <v>0</v>
       </c>
       <c r="EV31" s="12" t="s">
         <v>88</v>
@@ -24180,14 +24366,20 @@
         <v>88</v>
       </c>
       <c r="FG31" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FH31" s="12">
+        <v>0</v>
+      </c>
+      <c r="FI31" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="FH31" t="str">
+      <c r="FJ31" t="str">
         <f>Tabelle1!AV31</f>
         <v>Savage Shock Ultra</v>
       </c>
     </row>
-    <row r="32" spans="1:164" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:166" x14ac:dyDescent="0.25">
       <c r="A32" s="12" t="s">
         <v>88</v>
       </c>
@@ -24676,8 +24868,8 @@
       <c r="ET32" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="EU32" s="12" t="s">
-        <v>88</v>
+      <c r="EU32" s="12">
+        <v>0</v>
       </c>
       <c r="EV32" s="12" t="s">
         <v>88</v>
@@ -24713,14 +24905,20 @@
         <v>88</v>
       </c>
       <c r="FG32" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FH32" s="12">
+        <v>0</v>
+      </c>
+      <c r="FI32" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="FH32" t="str">
+      <c r="FJ32" t="str">
         <f>Tabelle1!AV32</f>
         <v>SR22</v>
       </c>
     </row>
-    <row r="33" spans="1:164" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:166" x14ac:dyDescent="0.25">
       <c r="A33" s="12" t="s">
         <v>88</v>
       </c>
@@ -25209,8 +25407,8 @@
       <c r="ET33" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="EU33" s="12" t="s">
-        <v>88</v>
+      <c r="EU33" s="12">
+        <v>0</v>
       </c>
       <c r="EV33" s="12" t="s">
         <v>88</v>
@@ -25246,14 +25444,20 @@
         <v>88</v>
       </c>
       <c r="FG33" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FH33" s="12">
+        <v>0</v>
+      </c>
+      <c r="FI33" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="FH33" t="str">
+      <c r="FJ33" t="str">
         <f>Tabelle1!AV33</f>
         <v>TBM 930</v>
       </c>
     </row>
-    <row r="34" spans="1:164" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:166" x14ac:dyDescent="0.25">
       <c r="A34" s="12" t="s">
         <v>88</v>
       </c>
@@ -25742,8 +25946,8 @@
       <c r="ET34" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="EU34" s="12" t="s">
-        <v>88</v>
+      <c r="EU34" s="12">
+        <v>0</v>
       </c>
       <c r="EV34" s="12" t="s">
         <v>88</v>
@@ -25779,14 +25983,20 @@
         <v>88</v>
       </c>
       <c r="FG34" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FH34" s="12">
+        <v>0</v>
+      </c>
+      <c r="FI34" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="FH34" t="str">
+      <c r="FJ34" t="str">
         <f>Tabelle1!AV34</f>
         <v>Vertigo</v>
       </c>
     </row>
-    <row r="35" spans="1:164" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:166" x14ac:dyDescent="0.25">
       <c r="A35" s="12" t="s">
         <v>88</v>
       </c>
@@ -26275,8 +26485,8 @@
       <c r="ET35" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="EU35" s="12" t="s">
-        <v>88</v>
+      <c r="EU35" s="12">
+        <v>0</v>
       </c>
       <c r="EV35" s="12" t="s">
         <v>88</v>
@@ -26312,14 +26522,20 @@
         <v>88</v>
       </c>
       <c r="FG35" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FH35" s="12">
+        <v>0</v>
+      </c>
+      <c r="FI35" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="FH35" t="str">
+      <c r="FJ35" t="str">
         <f>Tabelle1!AV35</f>
         <v>VL3</v>
       </c>
     </row>
-    <row r="36" spans="1:164" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:166" x14ac:dyDescent="0.25">
       <c r="A36" s="12" t="s">
         <v>88</v>
       </c>
@@ -26808,8 +27024,8 @@
       <c r="ET36" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="EU36" s="12" t="s">
-        <v>88</v>
+      <c r="EU36" s="12">
+        <v>0</v>
       </c>
       <c r="EV36" s="12" t="s">
         <v>88</v>
@@ -26845,14 +27061,20 @@
         <v>88</v>
       </c>
       <c r="FG36" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FH36" s="12">
+        <v>0</v>
+      </c>
+      <c r="FI36" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="FH36" t="str">
+      <c r="FJ36" t="str">
         <f>Tabelle1!AV36</f>
         <v>Volocity</v>
       </c>
     </row>
-    <row r="37" spans="1:164" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:166" x14ac:dyDescent="0.25">
       <c r="A37" s="12" t="s">
         <v>88</v>
       </c>
@@ -27341,8 +27563,8 @@
       <c r="ET37" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="EU37" s="12" t="s">
-        <v>88</v>
+      <c r="EU37" s="12">
+        <v>0</v>
       </c>
       <c r="EV37" s="12" t="s">
         <v>88</v>
@@ -27378,14 +27600,20 @@
         <v>88</v>
       </c>
       <c r="FG37" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FH37" s="12">
+        <v>0</v>
+      </c>
+      <c r="FI37" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="FH37" t="str">
+      <c r="FJ37" t="str">
         <f>Tabelle1!AV37</f>
         <v>NXCub</v>
       </c>
     </row>
-    <row r="38" spans="1:164" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:166" x14ac:dyDescent="0.25">
       <c r="A38" s="12" t="s">
         <v>88</v>
       </c>
@@ -27874,8 +28102,8 @@
       <c r="ET38" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="EU38" s="12" t="s">
-        <v>88</v>
+      <c r="EU38" s="12">
+        <v>0</v>
       </c>
       <c r="EV38" s="12" t="s">
         <v>88</v>
@@ -27911,14 +28139,20 @@
         <v>88</v>
       </c>
       <c r="FG38" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FH38" s="12">
+        <v>0</v>
+      </c>
+      <c r="FI38" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="FH38" t="str">
+      <c r="FJ38" t="str">
         <f>Tabelle1!AV38</f>
         <v>XCub</v>
       </c>
     </row>
-    <row r="39" spans="1:164" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:166" x14ac:dyDescent="0.25">
       <c r="A39" s="12" t="s">
         <v>88</v>
       </c>
@@ -28407,8 +28641,8 @@
       <c r="ET39" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="EU39" s="12" t="s">
-        <v>88</v>
+      <c r="EU39" s="12">
+        <v>0</v>
       </c>
       <c r="EV39" s="12" t="s">
         <v>88</v>
@@ -28444,14 +28678,20 @@
         <v>88</v>
       </c>
       <c r="FG39" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FH39" s="12">
+        <v>0</v>
+      </c>
+      <c r="FI39" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="FH39" t="str">
+      <c r="FJ39" t="str">
         <f>Tabelle1!AV39</f>
         <v>SWS Kodiak 100 II</v>
       </c>
     </row>
-    <row r="40" spans="1:164" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:166" x14ac:dyDescent="0.25">
       <c r="A40" s="12" t="s">
         <v>88</v>
       </c>
@@ -28940,8 +29180,8 @@
       <c r="ET40" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="EU40" s="12" t="s">
-        <v>88</v>
+      <c r="EU40" s="12">
+        <v>0</v>
       </c>
       <c r="EV40" s="12" t="s">
         <v>88</v>
@@ -28977,14 +29217,20 @@
         <v>88</v>
       </c>
       <c r="FG40" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FH40" s="12">
+        <v>0</v>
+      </c>
+      <c r="FI40" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="FH40" t="str">
+      <c r="FJ40" t="str">
         <f>Tabelle1!AV40</f>
         <v>Generic Glider</v>
       </c>
     </row>
-    <row r="41" spans="1:164" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:166" x14ac:dyDescent="0.25">
       <c r="A41" s="12" t="s">
         <v>88</v>
       </c>
@@ -29473,8 +29719,8 @@
       <c r="ET41" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="EU41" s="12" t="s">
-        <v>88</v>
+      <c r="EU41" s="12">
+        <v>1</v>
       </c>
       <c r="EV41" s="12" t="s">
         <v>88</v>
@@ -29510,9 +29756,15 @@
         <v>88</v>
       </c>
       <c r="FG41" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="FH41" s="12">
+        <v>1</v>
+      </c>
+      <c r="FI41" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="FH41" t="str">
+      <c r="FJ41" t="str">
         <f>Tabelle1!AV41</f>
         <v>Generic Heli Turbine</v>
       </c>

</xml_diff>